<commit_message>
Add xls to xml tool;add sample logic config excel file(Player.xlsx)
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Struct\Class\Player\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\python_project\xls2xml\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14445"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14445" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Property" sheetId="1" r:id="rId1"/>
+    <sheet name="Record_BagItemList" sheetId="3" r:id="rId2"/>
+    <sheet name="Record_PetList" sheetId="5" r:id="rId3"/>
+    <sheet name="Component" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="87">
   <si>
     <t>列3</t>
   </si>
@@ -284,252 +286,6 @@
     <t>列18</t>
   </si>
   <si>
-    <t>列19</t>
-  </si>
-  <si>
-    <t>列20</t>
-  </si>
-  <si>
-    <t>列21</t>
-  </si>
-  <si>
-    <t>列22</t>
-  </si>
-  <si>
-    <t>列23</t>
-  </si>
-  <si>
-    <t>列24</t>
-  </si>
-  <si>
-    <t>列25</t>
-  </si>
-  <si>
-    <t>列26</t>
-  </si>
-  <si>
-    <t>列27</t>
-  </si>
-  <si>
-    <t>列28</t>
-  </si>
-  <si>
-    <t>列29</t>
-  </si>
-  <si>
-    <t>列30</t>
-  </si>
-  <si>
-    <t>列31</t>
-  </si>
-  <si>
-    <t>列32</t>
-  </si>
-  <si>
-    <t>列33</t>
-  </si>
-  <si>
-    <t>列34</t>
-  </si>
-  <si>
-    <t>列35</t>
-  </si>
-  <si>
-    <t>列36</t>
-  </si>
-  <si>
-    <t>列37</t>
-  </si>
-  <si>
-    <t>列38</t>
-  </si>
-  <si>
-    <t>列39</t>
-  </si>
-  <si>
-    <t>列40</t>
-  </si>
-  <si>
-    <t>列41</t>
-  </si>
-  <si>
-    <t>列42</t>
-  </si>
-  <si>
-    <t>列43</t>
-  </si>
-  <si>
-    <t>列44</t>
-  </si>
-  <si>
-    <t>列45</t>
-  </si>
-  <si>
-    <t>列46</t>
-  </si>
-  <si>
-    <t>列47</t>
-  </si>
-  <si>
-    <t>列48</t>
-  </si>
-  <si>
-    <t>列49</t>
-  </si>
-  <si>
-    <t>列50</t>
-  </si>
-  <si>
-    <t>列51</t>
-  </si>
-  <si>
-    <t>列52</t>
-  </si>
-  <si>
-    <t>列53</t>
-  </si>
-  <si>
-    <t>列54</t>
-  </si>
-  <si>
-    <t>列55</t>
-  </si>
-  <si>
-    <t>列56</t>
-  </si>
-  <si>
-    <t>列57</t>
-  </si>
-  <si>
-    <t>列58</t>
-  </si>
-  <si>
-    <t>列59</t>
-  </si>
-  <si>
-    <t>列60</t>
-  </si>
-  <si>
-    <t>列61</t>
-  </si>
-  <si>
-    <t>列62</t>
-  </si>
-  <si>
-    <t>列63</t>
-  </si>
-  <si>
-    <t>列64</t>
-  </si>
-  <si>
-    <t>列65</t>
-  </si>
-  <si>
-    <t>列66</t>
-  </si>
-  <si>
-    <t>列67</t>
-  </si>
-  <si>
-    <t>列68</t>
-  </si>
-  <si>
-    <t>列69</t>
-  </si>
-  <si>
-    <t>列70</t>
-  </si>
-  <si>
-    <t>列71</t>
-  </si>
-  <si>
-    <t>列72</t>
-  </si>
-  <si>
-    <t>列73</t>
-  </si>
-  <si>
-    <t>列74</t>
-  </si>
-  <si>
-    <t>列75</t>
-  </si>
-  <si>
-    <t>列76</t>
-  </si>
-  <si>
-    <t>列77</t>
-  </si>
-  <si>
-    <t>列78</t>
-  </si>
-  <si>
-    <t>列79</t>
-  </si>
-  <si>
-    <t>列80</t>
-  </si>
-  <si>
-    <t>列81</t>
-  </si>
-  <si>
-    <t>列82</t>
-  </si>
-  <si>
-    <t>列83</t>
-  </si>
-  <si>
-    <t>列84</t>
-  </si>
-  <si>
-    <t>列85</t>
-  </si>
-  <si>
-    <t>列86</t>
-  </si>
-  <si>
-    <t>列87</t>
-  </si>
-  <si>
-    <t>列88</t>
-  </si>
-  <si>
-    <t>列89</t>
-  </si>
-  <si>
-    <t>列90</t>
-  </si>
-  <si>
-    <t>列91</t>
-  </si>
-  <si>
-    <t>列92</t>
-  </si>
-  <si>
-    <t>列93</t>
-  </si>
-  <si>
-    <t>列94</t>
-  </si>
-  <si>
-    <t>列95</t>
-  </si>
-  <si>
-    <t>列96</t>
-  </si>
-  <si>
-    <t>列97</t>
-  </si>
-  <si>
-    <t>列98</t>
-  </si>
-  <si>
-    <t>列99</t>
-  </si>
-  <si>
-    <t>列100</t>
-  </si>
-  <si>
     <t>BagItemList</t>
   </si>
   <si>
@@ -549,6 +305,10 @@
   </si>
   <si>
     <t>GUID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PetList</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -760,34 +520,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:I24" tableType="xml" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:I24" tableType="xml" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" connectionId="1">
   <autoFilter ref="A1:I24"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="Id" name="Id" dataDxfId="10">
+    <tableColumn id="1" uniqueName="Id" name="Id" dataDxfId="8">
       <xmlColumnPr mapId="1" xpath="/XML/Propertys/Property/@Id" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Type" name="Type" dataDxfId="9">
+    <tableColumn id="2" uniqueName="Type" name="Type" dataDxfId="7">
       <xmlColumnPr mapId="1" xpath="/XML/Propertys/Property/@Type" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Public" name="Public" dataDxfId="8">
+    <tableColumn id="3" uniqueName="Public" name="Public" dataDxfId="6">
       <xmlColumnPr mapId="1" xpath="/XML/Propertys/Property/@Public" xmlDataType="boolean"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Private" name="Private" dataDxfId="7">
+    <tableColumn id="4" uniqueName="Private" name="Private" dataDxfId="5">
       <xmlColumnPr mapId="1" xpath="/XML/Propertys/Property/@Private" xmlDataType="boolean"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Save" name="Save" dataDxfId="6">
+    <tableColumn id="5" uniqueName="Save" name="Save" dataDxfId="4">
       <xmlColumnPr mapId="1" xpath="/XML/Propertys/Property/@Save" xmlDataType="boolean"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Index" name="Index" dataDxfId="5">
+    <tableColumn id="6" uniqueName="Index" name="Index" dataDxfId="3">
       <xmlColumnPr mapId="1" xpath="/XML/Propertys/Property/@Index" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="SaveInterval" name="SaveInterval" dataDxfId="4">
+    <tableColumn id="7" uniqueName="SaveInterval" name="SaveInterval" dataDxfId="2">
       <xmlColumnPr mapId="1" xpath="/XML/Propertys/Property/@SaveInterval" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="RelationValue" name="RelationValue" dataDxfId="3">
+    <tableColumn id="8" uniqueName="RelationValue" name="RelationValue" dataDxfId="1">
       <xmlColumnPr mapId="1" xpath="/XML/Propertys/Property/@RelationValue" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="Desc" name="Desc" dataDxfId="2">
+    <tableColumn id="9" uniqueName="Desc" name="Desc" dataDxfId="0">
       <xmlColumnPr mapId="1" xpath="/XML/Propertys/Property/@Desc" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -796,9 +556,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表1_4" displayName="表1_4" ref="A1:DF33" totalsRowShown="0">
-  <autoFilter ref="A1:DF33"/>
-  <tableColumns count="110">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表1_4" displayName="表1_4" ref="A1:AB3" totalsRowShown="0">
+  <autoFilter ref="A1:AB3"/>
+  <tableColumns count="28">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Row"/>
     <tableColumn id="3" name="Col"/>
@@ -827,88 +587,43 @@
     <tableColumn id="38" name="列16"/>
     <tableColumn id="39" name="列17"/>
     <tableColumn id="40" name="列18"/>
-    <tableColumn id="41" name="列19"/>
-    <tableColumn id="42" name="列20"/>
-    <tableColumn id="43" name="列21"/>
-    <tableColumn id="44" name="列22"/>
-    <tableColumn id="45" name="列23"/>
-    <tableColumn id="46" name="列24"/>
-    <tableColumn id="47" name="列25"/>
-    <tableColumn id="48" name="列26"/>
-    <tableColumn id="49" name="列27"/>
-    <tableColumn id="50" name="列28"/>
-    <tableColumn id="51" name="列29"/>
-    <tableColumn id="52" name="列30"/>
-    <tableColumn id="53" name="列31"/>
-    <tableColumn id="54" name="列32"/>
-    <tableColumn id="55" name="列33"/>
-    <tableColumn id="56" name="列34"/>
-    <tableColumn id="57" name="列35"/>
-    <tableColumn id="58" name="列36"/>
-    <tableColumn id="59" name="列37"/>
-    <tableColumn id="60" name="列38"/>
-    <tableColumn id="61" name="列39"/>
-    <tableColumn id="62" name="列40"/>
-    <tableColumn id="63" name="列41"/>
-    <tableColumn id="64" name="列42"/>
-    <tableColumn id="65" name="列43"/>
-    <tableColumn id="66" name="列44"/>
-    <tableColumn id="67" name="列45"/>
-    <tableColumn id="68" name="列46"/>
-    <tableColumn id="69" name="列47"/>
-    <tableColumn id="70" name="列48"/>
-    <tableColumn id="71" name="列49"/>
-    <tableColumn id="72" name="列50"/>
-    <tableColumn id="73" name="列51"/>
-    <tableColumn id="74" name="列52"/>
-    <tableColumn id="75" name="列53"/>
-    <tableColumn id="76" name="列54"/>
-    <tableColumn id="77" name="列55"/>
-    <tableColumn id="78" name="列56"/>
-    <tableColumn id="79" name="列57"/>
-    <tableColumn id="80" name="列58"/>
-    <tableColumn id="81" name="列59"/>
-    <tableColumn id="82" name="列60"/>
-    <tableColumn id="83" name="列61"/>
-    <tableColumn id="84" name="列62"/>
-    <tableColumn id="85" name="列63"/>
-    <tableColumn id="86" name="列64"/>
-    <tableColumn id="87" name="列65"/>
-    <tableColumn id="88" name="列66"/>
-    <tableColumn id="89" name="列67"/>
-    <tableColumn id="90" name="列68"/>
-    <tableColumn id="91" name="列69"/>
-    <tableColumn id="92" name="列70"/>
-    <tableColumn id="93" name="列71"/>
-    <tableColumn id="94" name="列72"/>
-    <tableColumn id="95" name="列73"/>
-    <tableColumn id="96" name="列74"/>
-    <tableColumn id="97" name="列75"/>
-    <tableColumn id="98" name="列76"/>
-    <tableColumn id="99" name="列77"/>
-    <tableColumn id="100" name="列78"/>
-    <tableColumn id="101" name="列79"/>
-    <tableColumn id="102" name="列80"/>
-    <tableColumn id="103" name="列81"/>
-    <tableColumn id="104" name="列82"/>
-    <tableColumn id="105" name="列83"/>
-    <tableColumn id="106" name="列84"/>
-    <tableColumn id="107" name="列85"/>
-    <tableColumn id="108" name="列86"/>
-    <tableColumn id="109" name="列87"/>
-    <tableColumn id="110" name="列88"/>
-    <tableColumn id="111" name="列89"/>
-    <tableColumn id="112" name="列90"/>
-    <tableColumn id="113" name="列91"/>
-    <tableColumn id="114" name="列92"/>
-    <tableColumn id="115" name="列93"/>
-    <tableColumn id="116" name="列94"/>
-    <tableColumn id="117" name="列95"/>
-    <tableColumn id="118" name="列96"/>
-    <tableColumn id="119" name="列97"/>
-    <tableColumn id="120" name="列98"/>
-    <tableColumn id="121" name="列99"/>
-    <tableColumn id="122" name="列100"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_43" displayName="表1_43" ref="A1:AB3" totalsRowShown="0">
+  <autoFilter ref="A1:AB3"/>
+  <tableColumns count="28">
+    <tableColumn id="1" name="Id"/>
+    <tableColumn id="2" name="Row"/>
+    <tableColumn id="3" name="Col"/>
+    <tableColumn id="4" name="Public"/>
+    <tableColumn id="5" name="Private"/>
+    <tableColumn id="6" name="Save"/>
+    <tableColumn id="7" name="Index"/>
+    <tableColumn id="8" name="SaveInterval"/>
+    <tableColumn id="9" name="RelationValue"/>
+    <tableColumn id="10" name="Desc"/>
+    <tableColumn id="13" name="ItemID"/>
+    <tableColumn id="14" name="GUID"/>
+    <tableColumn id="15" name="列3"/>
+    <tableColumn id="16" name="列4"/>
+    <tableColumn id="17" name="列5"/>
+    <tableColumn id="18" name="列6"/>
+    <tableColumn id="19" name="列7"/>
+    <tableColumn id="20" name="列8"/>
+    <tableColumn id="21" name="列9"/>
+    <tableColumn id="22" name="列10"/>
+    <tableColumn id="23" name="列11"/>
+    <tableColumn id="24" name="列12"/>
+    <tableColumn id="25" name="列13"/>
+    <tableColumn id="26" name="列14"/>
+    <tableColumn id="37" name="列15"/>
+    <tableColumn id="38" name="列16"/>
+    <tableColumn id="39" name="列17"/>
+    <tableColumn id="40" name="列18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1179,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1913,17 +1628,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DF32"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:110" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>166</v>
+        <v>84</v>
       </c>
       <c r="B1" t="s">
         <v>68</v>
@@ -1956,7 +1674,7 @@
         <v>70</v>
       </c>
       <c r="L1" t="s">
-        <v>167</v>
+        <v>85</v>
       </c>
       <c r="M1" t="s">
         <v>0</v>
@@ -2006,256 +1724,10 @@
       <c r="AB1" t="s">
         <v>79</v>
       </c>
-      <c r="AC1" t="s">
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>99</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>103</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>104</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>105</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>106</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>107</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>108</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>109</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>110</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>111</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>112</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>113</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>114</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>115</v>
-      </c>
-      <c r="BM1" t="s">
-        <v>116</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>117</v>
-      </c>
-      <c r="BO1" t="s">
-        <v>118</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>119</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>120</v>
-      </c>
-      <c r="BR1" t="s">
-        <v>121</v>
-      </c>
-      <c r="BS1" t="s">
-        <v>122</v>
-      </c>
-      <c r="BT1" t="s">
-        <v>123</v>
-      </c>
-      <c r="BU1" t="s">
-        <v>124</v>
-      </c>
-      <c r="BV1" t="s">
-        <v>125</v>
-      </c>
-      <c r="BW1" t="s">
-        <v>126</v>
-      </c>
-      <c r="BX1" t="s">
-        <v>127</v>
-      </c>
-      <c r="BY1" t="s">
-        <v>128</v>
-      </c>
-      <c r="BZ1" t="s">
-        <v>129</v>
-      </c>
-      <c r="CA1" t="s">
-        <v>130</v>
-      </c>
-      <c r="CB1" t="s">
-        <v>131</v>
-      </c>
-      <c r="CC1" t="s">
-        <v>132</v>
-      </c>
-      <c r="CD1" t="s">
-        <v>133</v>
-      </c>
-      <c r="CE1" t="s">
-        <v>134</v>
-      </c>
-      <c r="CF1" t="s">
-        <v>135</v>
-      </c>
-      <c r="CG1" t="s">
-        <v>136</v>
-      </c>
-      <c r="CH1" t="s">
-        <v>137</v>
-      </c>
-      <c r="CI1" t="s">
-        <v>138</v>
-      </c>
-      <c r="CJ1" t="s">
-        <v>139</v>
-      </c>
-      <c r="CK1" t="s">
-        <v>140</v>
-      </c>
-      <c r="CL1" t="s">
-        <v>141</v>
-      </c>
-      <c r="CM1" t="s">
-        <v>142</v>
-      </c>
-      <c r="CN1" t="s">
-        <v>143</v>
-      </c>
-      <c r="CO1" t="s">
-        <v>144</v>
-      </c>
-      <c r="CP1" t="s">
-        <v>145</v>
-      </c>
-      <c r="CQ1" t="s">
-        <v>146</v>
-      </c>
-      <c r="CR1" t="s">
-        <v>147</v>
-      </c>
-      <c r="CS1" t="s">
-        <v>148</v>
-      </c>
-      <c r="CT1" t="s">
-        <v>149</v>
-      </c>
-      <c r="CU1" t="s">
-        <v>150</v>
-      </c>
-      <c r="CV1" t="s">
-        <v>151</v>
-      </c>
-      <c r="CW1" t="s">
-        <v>152</v>
-      </c>
-      <c r="CX1" t="s">
-        <v>153</v>
-      </c>
-      <c r="CY1" t="s">
-        <v>154</v>
-      </c>
-      <c r="CZ1" t="s">
-        <v>155</v>
-      </c>
-      <c r="DA1" t="s">
-        <v>156</v>
-      </c>
-      <c r="DB1" t="s">
-        <v>157</v>
-      </c>
-      <c r="DC1" t="s">
-        <v>158</v>
-      </c>
-      <c r="DD1" t="s">
-        <v>159</v>
-      </c>
-      <c r="DE1" t="s">
-        <v>160</v>
-      </c>
-      <c r="DF1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:110" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="B2">
         <v>211</v>
@@ -2282,202 +1754,70 @@
         <v>42</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>163</v>
+        <v>81</v>
       </c>
       <c r="K2" t="s">
-        <v>164</v>
+        <v>82</v>
       </c>
       <c r="L2" t="s">
-        <v>165</v>
+        <v>83</v>
       </c>
       <c r="M2" t="s">
-        <v>165</v>
+        <v>83</v>
       </c>
       <c r="N2" t="s">
-        <v>165</v>
+        <v>83</v>
       </c>
       <c r="O2" t="s">
-        <v>165</v>
+        <v>83</v>
       </c>
       <c r="P2" t="s">
-        <v>165</v>
+        <v>83</v>
       </c>
       <c r="Q2" t="s">
-        <v>165</v>
+        <v>83</v>
       </c>
       <c r="R2" t="s">
-        <v>165</v>
+        <v>83</v>
       </c>
       <c r="S2" t="s">
-        <v>165</v>
+        <v>83</v>
       </c>
       <c r="T2" t="s">
-        <v>165</v>
+        <v>83</v>
       </c>
       <c r="U2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="3" spans="1:110" x14ac:dyDescent="0.15">
-      <c r="A3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:110" x14ac:dyDescent="0.15">
-      <c r="A4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:110" x14ac:dyDescent="0.15">
-      <c r="A5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:110" x14ac:dyDescent="0.15">
-      <c r="A6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:110" x14ac:dyDescent="0.15">
-      <c r="A7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:110" x14ac:dyDescent="0.15">
-      <c r="A8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:110" x14ac:dyDescent="0.15">
-      <c r="A9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:110" x14ac:dyDescent="0.15">
-      <c r="A10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:110" x14ac:dyDescent="0.15">
-      <c r="A11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:110" x14ac:dyDescent="0.15">
-      <c r="A12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:110" x14ac:dyDescent="0.15">
-      <c r="A13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:110" x14ac:dyDescent="0.15">
-      <c r="A14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:110" x14ac:dyDescent="0.15">
-      <c r="A15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:110" x14ac:dyDescent="0.15">
-      <c r="A16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
+        <v>83</v>
+      </c>
+      <c r="V2" t="s">
+        <v>66</v>
+      </c>
+      <c r="W2" t="s">
+        <v>66</v>
+      </c>
+      <c r="X2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="3">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
+  <dataValidations count="2">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576 E1:E1048576 F1:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2486,4 +1826,221 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T1" t="s">
+        <v>71</v>
+      </c>
+      <c r="U1" t="s">
+        <v>72</v>
+      </c>
+      <c r="V1" t="s">
+        <v>73</v>
+      </c>
+      <c r="W1" t="s">
+        <v>74</v>
+      </c>
+      <c r="X1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2">
+        <v>211</v>
+      </c>
+      <c r="C2">
+        <v>18</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M2" t="s">
+        <v>66</v>
+      </c>
+      <c r="N2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O2" t="s">
+        <v>66</v>
+      </c>
+      <c r="P2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>66</v>
+      </c>
+      <c r="R2" t="s">
+        <v>66</v>
+      </c>
+      <c r="S2" t="s">
+        <v>66</v>
+      </c>
+      <c r="T2" t="s">
+        <v>66</v>
+      </c>
+      <c r="U2" t="s">
+        <v>66</v>
+      </c>
+      <c r="V2" t="s">
+        <v>66</v>
+      </c>
+      <c r="W2" t="s">
+        <v>66</v>
+      </c>
+      <c r="X2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:F1048576">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed bug for broadcast property add modified property value in client
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
@@ -414,7 +414,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="221">
   <si>
     <t>Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1156,6 +1156,9 @@
   <si>
     <t>TaskStatus</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoadPropertyFinish</t>
   </si>
 </sst>
 </file>
@@ -1293,8 +1296,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:I73" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:I73"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:I74" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:I74"/>
   <tableColumns count="9">
     <tableColumn id="1" uniqueName="Id" name="Id">
       <xmlColumnPr mapId="1" xpath="/Propertys/Property/@Id" xmlDataType="string"/>
@@ -1761,15 +1764,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:I74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+      <selection activeCell="H75" sqref="H75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.875" customWidth="1"/>
     <col min="2" max="2" width="8.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.625" bestFit="1" customWidth="1"/>
@@ -3881,11 +3884,38 @@
       </c>
       <c r="I73" s="1"/>
     </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A74" t="s">
+        <v>220</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C74" t="b">
+        <v>0</v>
+      </c>
+      <c r="D74" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" t="b">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
add components config; modify xls2xml.exe for components
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Struct\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\NoahGameFrame\_Out\Server\NFDataCfg\Excel_Struct\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27315" windowHeight="14835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27315" windowHeight="14835" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Property" sheetId="1" r:id="rId1"/>
@@ -414,7 +414,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="227">
   <si>
     <t>Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1159,6 +1159,29 @@
   </si>
   <si>
     <t>LoadPropertyFinish</t>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Language</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lua</t>
+  </si>
+  <si>
+    <t>测试组件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1251,7 +1274,11 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1496,6 +1523,19 @@
     <tableColumn id="10" name="Desc"/>
     <tableColumn id="13" name="TaskID"/>
     <tableColumn id="14" name="TaskStatus"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="表1_46789" displayName="表1_46789" ref="A1:D2" totalsRowShown="0">
+  <autoFilter ref="A1:D2"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="9" name="Language"/>
+    <tableColumn id="2" name="Enable" dataDxfId="0"/>
+    <tableColumn id="10" name="Desc"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1766,7 +1806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="H75" sqref="H75"/>
     </sheetView>
   </sheetViews>
@@ -4805,7 +4845,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4920,15 +4960,60 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"lua,python,C#,js"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add drop item function when kill monster; Because EctypeModule is developing(Demand is not clear, still thinking), so cannot draw drop items right now, :)
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
@@ -16,12 +16,13 @@
     <sheet name="Record_PlayerViewItem" sheetId="2" r:id="rId2"/>
     <sheet name="Record_CommPropertyValue" sheetId="3" r:id="rId3"/>
     <sheet name="Record_BagItemList" sheetId="4" r:id="rId4"/>
-    <sheet name="Record_DropItemList" sheetId="10" r:id="rId5"/>
-    <sheet name="Record_SkillTable" sheetId="5" r:id="rId6"/>
-    <sheet name="Record_TaskMonsterList" sheetId="6" r:id="rId7"/>
-    <sheet name="Record_TaskList" sheetId="7" r:id="rId8"/>
-    <sheet name="Record_PvpList" sheetId="9" r:id="rId9"/>
-    <sheet name="Component" sheetId="8" r:id="rId10"/>
+    <sheet name="Record_EctypeList" sheetId="11" r:id="rId5"/>
+    <sheet name="Record_DropItemList" sheetId="10" r:id="rId6"/>
+    <sheet name="Record_SkillTable" sheetId="5" r:id="rId7"/>
+    <sheet name="Record_TaskMonsterList" sheetId="6" r:id="rId8"/>
+    <sheet name="Record_TaskList" sheetId="7" r:id="rId9"/>
+    <sheet name="Record_PvpList" sheetId="9" r:id="rId10"/>
+    <sheet name="Component" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -219,6 +220,58 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
+          <t>关卡ID</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">是否通关
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>通过时的星级</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>pengbo.yang</author>
+    <author>杨鹏博</author>
+  </authors>
+  <commentList>
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
           <t>怪物GUID</t>
         </r>
       </text>
@@ -265,68 +318,6 @@
 0 初始状态
 1 可以领
 2 领过了</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>pengbo.yang</author>
-  </authors>
-  <commentList>
-    <comment ref="L1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>物品配置ID</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>强化等级</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>镶嵌宝石，逗号分隔</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>附魔等级</t>
         </r>
       </text>
     </comment>
@@ -428,6 +419,32 @@
         </r>
       </text>
     </comment>
+    <comment ref="N1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>镶嵌宝石，逗号分隔</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>附魔等级</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -468,8 +485,44 @@
 </comments>
 </file>
 
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>pengbo.yang</author>
+  </authors>
+  <commentList>
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>物品配置ID</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>强化等级</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="217">
   <si>
     <t>Id</t>
   </si>
@@ -1114,6 +1167,30 @@
   </si>
   <si>
     <t>object</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>EctypeList</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>副本列表</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>EctypeID</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsPass</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Star</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -3955,6 +4032,133 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="10" max="10" width="18.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>198</v>
+      </c>
+      <c r="M1" t="s">
+        <v>200</v>
+      </c>
+      <c r="N1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="L2" t="s">
+        <v>199</v>
+      </c>
+      <c r="M2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:F2">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C2">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L2 M2">
+      <formula1>"int,float,string,object"</formula1>
+    </dataValidation>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="L1 M1"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2">
+      <formula1>"int,float,string,object"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -4643,9 +4847,141 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="16.125" customWidth="1"/>
+    <col min="2" max="3" width="7.125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="11.625" customWidth="1"/>
+    <col min="8" max="8" width="9.375" customWidth="1"/>
+    <col min="9" max="9" width="17.75" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.75" customWidth="1"/>
+    <col min="13" max="13" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M1" t="s">
+        <v>215</v>
+      </c>
+      <c r="N1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2">
+        <v>128</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="M2" t="s">
+        <v>214</v>
+      </c>
+      <c r="N2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <dataValidations count="4">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="L1:M1048576"/>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G42">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:F1048576">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -4780,7 +5116,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -4914,7 +5250,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -5051,7 +5387,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
@@ -5175,131 +5511,4 @@
   <headerFooter alignWithMargins="0"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="10" max="10" width="18.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>198</v>
-      </c>
-      <c r="M1" t="s">
-        <v>200</v>
-      </c>
-      <c r="N1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B2">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="L2" t="s">
-        <v>199</v>
-      </c>
-      <c r="M2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:F2">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C2">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L2 M2">
-      <formula1>"int,float,string,object"</formula1>
-    </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="L1 M1"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2">
-      <formula1>"int,float,string,object"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
change player property RoleName->Name
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8460" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8460" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Property" sheetId="1" r:id="rId1"/>
@@ -554,9 +554,6 @@
     <t>Desc</t>
   </si>
   <si>
-    <t>RoleName</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
@@ -1191,6 +1188,10 @@
   </si>
   <si>
     <t>Star</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1643,8 +1644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1694,11 +1695,11 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
@@ -1718,1298 +1719,1298 @@
         <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" t="b">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" t="b">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="b">
-        <v>1</v>
-      </c>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F15" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" t="b">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F17" t="b">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" t="b">
-        <v>1</v>
-      </c>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" t="b">
-        <v>1</v>
-      </c>
-      <c r="F18" t="b">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" t="b">
-        <v>1</v>
-      </c>
-      <c r="F19" t="b">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" t="b">
-        <v>1</v>
-      </c>
-      <c r="F20" t="b">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" t="b">
-        <v>1</v>
-      </c>
-      <c r="F21" t="b">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" t="b">
-        <v>1</v>
-      </c>
-      <c r="D22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" t="b">
-        <v>1</v>
-      </c>
-      <c r="F22" t="b">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E23" t="b">
-        <v>1</v>
-      </c>
-      <c r="F23" t="b">
-        <v>1</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" t="b">
-        <v>1</v>
-      </c>
-      <c r="D24" t="b">
-        <v>1</v>
-      </c>
-      <c r="E24" t="b">
-        <v>1</v>
-      </c>
-      <c r="F24" t="b">
-        <v>1</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" t="b">
-        <v>1</v>
-      </c>
-      <c r="D25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E25" t="b">
-        <v>1</v>
-      </c>
-      <c r="F25" t="b">
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J26" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" t="b">
-        <v>1</v>
-      </c>
-      <c r="D27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F27" t="b">
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J28" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F28" t="b">
-        <v>1</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" t="b">
+        <v>1</v>
+      </c>
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J29" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" t="b">
-        <v>1</v>
-      </c>
-      <c r="D29" t="b">
-        <v>1</v>
-      </c>
-      <c r="E29" t="b">
-        <v>1</v>
-      </c>
-      <c r="F29" t="b">
-        <v>1</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J30" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" t="b">
-        <v>1</v>
-      </c>
-      <c r="D30" t="b">
-        <v>1</v>
-      </c>
-      <c r="E30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F30" t="b">
-        <v>1</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" t="b">
+        <v>1</v>
+      </c>
+      <c r="E31" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" t="b">
-        <v>1</v>
-      </c>
-      <c r="D31" t="b">
-        <v>1</v>
-      </c>
-      <c r="E31" t="b">
-        <v>1</v>
-      </c>
-      <c r="F31" t="b">
-        <v>1</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" t="b">
+        <v>1</v>
+      </c>
+      <c r="E32" t="b">
+        <v>1</v>
+      </c>
+      <c r="F32" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" t="b">
-        <v>1</v>
-      </c>
-      <c r="D32" t="b">
-        <v>1</v>
-      </c>
-      <c r="E32" t="b">
-        <v>1</v>
-      </c>
-      <c r="F32" t="b">
-        <v>1</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33" t="b">
+        <v>1</v>
+      </c>
+      <c r="E33" t="b">
+        <v>1</v>
+      </c>
+      <c r="F33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" t="b">
-        <v>1</v>
-      </c>
-      <c r="D33" t="b">
-        <v>1</v>
-      </c>
-      <c r="E33" t="b">
-        <v>1</v>
-      </c>
-      <c r="F33" t="b">
-        <v>1</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J34" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" t="b">
-        <v>1</v>
-      </c>
-      <c r="D34" t="b">
-        <v>1</v>
-      </c>
-      <c r="E34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F34" t="b">
-        <v>1</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" t="b">
+        <v>1</v>
+      </c>
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" t="b">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J35" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" t="b">
-        <v>1</v>
-      </c>
-      <c r="D35" t="b">
-        <v>1</v>
-      </c>
-      <c r="E35" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" t="b">
-        <v>1</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" t="b">
+        <v>1</v>
+      </c>
+      <c r="D36" t="b">
+        <v>1</v>
+      </c>
+      <c r="E36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" t="b">
-        <v>1</v>
-      </c>
-      <c r="D36" t="b">
-        <v>1</v>
-      </c>
-      <c r="E36" t="b">
-        <v>1</v>
-      </c>
-      <c r="F36" t="b">
-        <v>1</v>
-      </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J37" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" t="b">
-        <v>1</v>
-      </c>
-      <c r="D37" t="b">
-        <v>1</v>
-      </c>
-      <c r="E37" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" t="b">
-        <v>1</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J38" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" t="b">
-        <v>1</v>
-      </c>
-      <c r="D38" t="b">
-        <v>1</v>
-      </c>
-      <c r="E38" t="b">
-        <v>1</v>
-      </c>
-      <c r="F38" t="b">
-        <v>1</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39" t="b">
+        <v>1</v>
+      </c>
+      <c r="E39" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J39" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C39" t="b">
-        <v>1</v>
-      </c>
-      <c r="D39" t="b">
-        <v>1</v>
-      </c>
-      <c r="E39" t="b">
-        <v>1</v>
-      </c>
-      <c r="F39" t="b">
-        <v>1</v>
-      </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J39" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40" t="b">
+        <v>1</v>
+      </c>
+      <c r="E40" t="b">
+        <v>1</v>
+      </c>
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J40" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C40" t="b">
-        <v>1</v>
-      </c>
-      <c r="D40" t="b">
-        <v>1</v>
-      </c>
-      <c r="E40" t="b">
-        <v>1</v>
-      </c>
-      <c r="F40" t="b">
-        <v>1</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" t="b">
+        <v>1</v>
+      </c>
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J41" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C41" t="b">
-        <v>1</v>
-      </c>
-      <c r="D41" t="b">
-        <v>1</v>
-      </c>
-      <c r="E41" t="b">
-        <v>1</v>
-      </c>
-      <c r="F41" t="b">
-        <v>1</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="b">
+        <v>1</v>
+      </c>
+      <c r="D42" t="b">
+        <v>1</v>
+      </c>
+      <c r="E42" t="b">
+        <v>1</v>
+      </c>
+      <c r="F42" t="b">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J42" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C42" t="b">
-        <v>1</v>
-      </c>
-      <c r="D42" t="b">
-        <v>1</v>
-      </c>
-      <c r="E42" t="b">
-        <v>1</v>
-      </c>
-      <c r="F42" t="b">
-        <v>1</v>
-      </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C43" t="b">
         <v>1</v>
@@ -3030,16 +3031,16 @@
         <v>0</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J43" s="1"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A44" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C44" t="b">
         <v>1</v>
@@ -3060,18 +3061,18 @@
         <v>0</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A45" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C45" t="b">
         <v>1</v>
@@ -3092,18 +3093,18 @@
         <v>0</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C46" t="b">
         <v>1</v>
@@ -3124,691 +3125,691 @@
         <v>0</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A47" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" t="b">
+        <v>1</v>
+      </c>
+      <c r="D47" t="b">
+        <v>1</v>
+      </c>
+      <c r="E47" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" t="b">
+        <v>1</v>
+      </c>
+      <c r="G47" s="3">
+        <v>0</v>
+      </c>
+      <c r="H47" s="3">
+        <v>0</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J47" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C47" t="b">
-        <v>1</v>
-      </c>
-      <c r="D47" t="b">
-        <v>1</v>
-      </c>
-      <c r="E47" t="b">
-        <v>1</v>
-      </c>
-      <c r="F47" t="b">
-        <v>1</v>
-      </c>
-      <c r="G47" s="3">
-        <v>0</v>
-      </c>
-      <c r="H47" s="3">
-        <v>0</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A48" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" t="b">
+        <v>1</v>
+      </c>
+      <c r="D48" t="b">
+        <v>1</v>
+      </c>
+      <c r="E48" t="b">
+        <v>1</v>
+      </c>
+      <c r="F48" t="b">
+        <v>1</v>
+      </c>
+      <c r="G48" s="3">
+        <v>0</v>
+      </c>
+      <c r="H48" s="3">
+        <v>0</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J48" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C48" t="b">
-        <v>1</v>
-      </c>
-      <c r="D48" t="b">
-        <v>1</v>
-      </c>
-      <c r="E48" t="b">
-        <v>1</v>
-      </c>
-      <c r="F48" t="b">
-        <v>1</v>
-      </c>
-      <c r="G48" s="3">
-        <v>0</v>
-      </c>
-      <c r="H48" s="3">
-        <v>0</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A49" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" t="b">
+        <v>1</v>
+      </c>
+      <c r="D49" t="b">
+        <v>1</v>
+      </c>
+      <c r="E49" t="b">
+        <v>1</v>
+      </c>
+      <c r="F49" t="b">
+        <v>1</v>
+      </c>
+      <c r="G49" s="3">
+        <v>0</v>
+      </c>
+      <c r="H49" s="3">
+        <v>0</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J49" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C49" t="b">
-        <v>1</v>
-      </c>
-      <c r="D49" t="b">
-        <v>1</v>
-      </c>
-      <c r="E49" t="b">
-        <v>1</v>
-      </c>
-      <c r="F49" t="b">
-        <v>1</v>
-      </c>
-      <c r="G49" s="3">
-        <v>0</v>
-      </c>
-      <c r="H49" s="3">
-        <v>0</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A50" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" t="b">
+        <v>1</v>
+      </c>
+      <c r="D50" t="b">
+        <v>1</v>
+      </c>
+      <c r="E50" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
+      <c r="G50" s="3">
+        <v>0</v>
+      </c>
+      <c r="H50" s="3">
+        <v>0</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J50" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C50" t="b">
-        <v>1</v>
-      </c>
-      <c r="D50" t="b">
-        <v>1</v>
-      </c>
-      <c r="E50" t="b">
-        <v>1</v>
-      </c>
-      <c r="F50" t="b">
-        <v>1</v>
-      </c>
-      <c r="G50" s="3">
-        <v>0</v>
-      </c>
-      <c r="H50" s="3">
-        <v>0</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A51" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" t="b">
+        <v>1</v>
+      </c>
+      <c r="D51" t="b">
+        <v>1</v>
+      </c>
+      <c r="E51" t="b">
+        <v>1</v>
+      </c>
+      <c r="F51" t="b">
+        <v>1</v>
+      </c>
+      <c r="G51" s="3">
+        <v>0</v>
+      </c>
+      <c r="H51" s="3">
+        <v>0</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J51" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C51" t="b">
-        <v>1</v>
-      </c>
-      <c r="D51" t="b">
-        <v>1</v>
-      </c>
-      <c r="E51" t="b">
-        <v>1</v>
-      </c>
-      <c r="F51" t="b">
-        <v>1</v>
-      </c>
-      <c r="G51" s="3">
-        <v>0</v>
-      </c>
-      <c r="H51" s="3">
-        <v>0</v>
-      </c>
-      <c r="I51" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J51" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" t="b">
+        <v>1</v>
+      </c>
+      <c r="D52" t="b">
+        <v>1</v>
+      </c>
+      <c r="E52" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" t="b">
+        <v>1</v>
+      </c>
+      <c r="G52" s="3">
+        <v>0</v>
+      </c>
+      <c r="H52" s="3">
+        <v>0</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J52" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C52" t="b">
-        <v>1</v>
-      </c>
-      <c r="D52" t="b">
-        <v>1</v>
-      </c>
-      <c r="E52" t="b">
-        <v>1</v>
-      </c>
-      <c r="F52" t="b">
-        <v>1</v>
-      </c>
-      <c r="G52" s="3">
-        <v>0</v>
-      </c>
-      <c r="H52" s="3">
-        <v>0</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J52" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A53" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" t="b">
+        <v>1</v>
+      </c>
+      <c r="D53" t="b">
+        <v>1</v>
+      </c>
+      <c r="E53" t="b">
+        <v>1</v>
+      </c>
+      <c r="F53" t="b">
+        <v>1</v>
+      </c>
+      <c r="G53" s="3">
+        <v>0</v>
+      </c>
+      <c r="H53" s="3">
+        <v>0</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J53" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C53" t="b">
-        <v>1</v>
-      </c>
-      <c r="D53" t="b">
-        <v>1</v>
-      </c>
-      <c r="E53" t="b">
-        <v>1</v>
-      </c>
-      <c r="F53" t="b">
-        <v>1</v>
-      </c>
-      <c r="G53" s="3">
-        <v>0</v>
-      </c>
-      <c r="H53" s="3">
-        <v>0</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J53" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A54" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" t="b">
+        <v>1</v>
+      </c>
+      <c r="D54" t="b">
+        <v>1</v>
+      </c>
+      <c r="E54" t="b">
+        <v>1</v>
+      </c>
+      <c r="F54" t="b">
+        <v>1</v>
+      </c>
+      <c r="G54" s="3">
+        <v>0</v>
+      </c>
+      <c r="H54" s="3">
+        <v>0</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J54" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C54" t="b">
-        <v>1</v>
-      </c>
-      <c r="D54" t="b">
-        <v>1</v>
-      </c>
-      <c r="E54" t="b">
-        <v>1</v>
-      </c>
-      <c r="F54" t="b">
-        <v>1</v>
-      </c>
-      <c r="G54" s="3">
-        <v>0</v>
-      </c>
-      <c r="H54" s="3">
-        <v>0</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A55" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" t="b">
+        <v>1</v>
+      </c>
+      <c r="D55" t="b">
+        <v>1</v>
+      </c>
+      <c r="E55" t="b">
+        <v>1</v>
+      </c>
+      <c r="F55" t="b">
+        <v>1</v>
+      </c>
+      <c r="G55" s="3">
+        <v>0</v>
+      </c>
+      <c r="H55" s="3">
+        <v>0</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J55" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C55" t="b">
-        <v>1</v>
-      </c>
-      <c r="D55" t="b">
-        <v>1</v>
-      </c>
-      <c r="E55" t="b">
-        <v>1</v>
-      </c>
-      <c r="F55" t="b">
-        <v>1</v>
-      </c>
-      <c r="G55" s="3">
-        <v>0</v>
-      </c>
-      <c r="H55" s="3">
-        <v>0</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J55" s="2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A56" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" t="b">
+        <v>1</v>
+      </c>
+      <c r="D56" t="b">
+        <v>1</v>
+      </c>
+      <c r="E56" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" t="b">
+        <v>1</v>
+      </c>
+      <c r="G56" s="3">
+        <v>0</v>
+      </c>
+      <c r="H56" s="3">
+        <v>0</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J56" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C56" t="b">
-        <v>1</v>
-      </c>
-      <c r="D56" t="b">
-        <v>1</v>
-      </c>
-      <c r="E56" t="b">
-        <v>1</v>
-      </c>
-      <c r="F56" t="b">
-        <v>1</v>
-      </c>
-      <c r="G56" s="3">
-        <v>0</v>
-      </c>
-      <c r="H56" s="3">
-        <v>0</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A57" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" t="b">
+        <v>1</v>
+      </c>
+      <c r="D57" t="b">
+        <v>1</v>
+      </c>
+      <c r="E57" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" t="b">
+        <v>1</v>
+      </c>
+      <c r="G57" s="3">
+        <v>0</v>
+      </c>
+      <c r="H57" s="3">
+        <v>0</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J57" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C57" t="b">
-        <v>1</v>
-      </c>
-      <c r="D57" t="b">
-        <v>1</v>
-      </c>
-      <c r="E57" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" t="b">
-        <v>1</v>
-      </c>
-      <c r="G57" s="3">
-        <v>0</v>
-      </c>
-      <c r="H57" s="3">
-        <v>0</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J57" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A58" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58" t="b">
+        <v>1</v>
+      </c>
+      <c r="D58" t="b">
+        <v>1</v>
+      </c>
+      <c r="E58" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" t="b">
+        <v>1</v>
+      </c>
+      <c r="G58" s="3">
+        <v>0</v>
+      </c>
+      <c r="H58" s="3">
+        <v>0</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J58" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C58" t="b">
-        <v>1</v>
-      </c>
-      <c r="D58" t="b">
-        <v>1</v>
-      </c>
-      <c r="E58" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" t="b">
-        <v>1</v>
-      </c>
-      <c r="G58" s="3">
-        <v>0</v>
-      </c>
-      <c r="H58" s="3">
-        <v>0</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A59" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59" t="b">
+        <v>1</v>
+      </c>
+      <c r="D59" t="b">
+        <v>1</v>
+      </c>
+      <c r="E59" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" t="b">
+        <v>1</v>
+      </c>
+      <c r="G59" s="3">
+        <v>0</v>
+      </c>
+      <c r="H59" s="3">
+        <v>0</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J59" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C59" t="b">
-        <v>1</v>
-      </c>
-      <c r="D59" t="b">
-        <v>1</v>
-      </c>
-      <c r="E59" t="b">
-        <v>1</v>
-      </c>
-      <c r="F59" t="b">
-        <v>1</v>
-      </c>
-      <c r="G59" s="3">
-        <v>0</v>
-      </c>
-      <c r="H59" s="3">
-        <v>0</v>
-      </c>
-      <c r="I59" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J59" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A60" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60" t="b">
+        <v>1</v>
+      </c>
+      <c r="D60" t="b">
+        <v>1</v>
+      </c>
+      <c r="E60" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" t="b">
+        <v>1</v>
+      </c>
+      <c r="G60" s="3">
+        <v>0</v>
+      </c>
+      <c r="H60" s="3">
+        <v>0</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J60" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C60" t="b">
-        <v>1</v>
-      </c>
-      <c r="D60" t="b">
-        <v>1</v>
-      </c>
-      <c r="E60" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" t="b">
-        <v>1</v>
-      </c>
-      <c r="G60" s="3">
-        <v>0</v>
-      </c>
-      <c r="H60" s="3">
-        <v>0</v>
-      </c>
-      <c r="I60" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J60" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A61" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" t="b">
+        <v>1</v>
+      </c>
+      <c r="D61" t="b">
+        <v>1</v>
+      </c>
+      <c r="E61" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" t="b">
+        <v>1</v>
+      </c>
+      <c r="G61" s="3">
+        <v>0</v>
+      </c>
+      <c r="H61" s="3">
+        <v>0</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J61" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C61" t="b">
-        <v>1</v>
-      </c>
-      <c r="D61" t="b">
-        <v>1</v>
-      </c>
-      <c r="E61" t="b">
-        <v>1</v>
-      </c>
-      <c r="F61" t="b">
-        <v>1</v>
-      </c>
-      <c r="G61" s="3">
-        <v>0</v>
-      </c>
-      <c r="H61" s="3">
-        <v>0</v>
-      </c>
-      <c r="I61" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J61" s="2" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A62" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62" t="b">
+        <v>1</v>
+      </c>
+      <c r="D62" t="b">
+        <v>1</v>
+      </c>
+      <c r="E62" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" t="b">
+        <v>1</v>
+      </c>
+      <c r="G62" s="3">
+        <v>0</v>
+      </c>
+      <c r="H62" s="3">
+        <v>0</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J62" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C62" t="b">
-        <v>1</v>
-      </c>
-      <c r="D62" t="b">
-        <v>1</v>
-      </c>
-      <c r="E62" t="b">
-        <v>1</v>
-      </c>
-      <c r="F62" t="b">
-        <v>1</v>
-      </c>
-      <c r="G62" s="3">
-        <v>0</v>
-      </c>
-      <c r="H62" s="3">
-        <v>0</v>
-      </c>
-      <c r="I62" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J62" s="2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A63" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" t="b">
+        <v>1</v>
+      </c>
+      <c r="D63" t="b">
+        <v>1</v>
+      </c>
+      <c r="E63" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" t="b">
+        <v>1</v>
+      </c>
+      <c r="G63" s="3">
+        <v>0</v>
+      </c>
+      <c r="H63" s="3">
+        <v>0</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J63" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C63" t="b">
-        <v>1</v>
-      </c>
-      <c r="D63" t="b">
-        <v>1</v>
-      </c>
-      <c r="E63" t="b">
-        <v>1</v>
-      </c>
-      <c r="F63" t="b">
-        <v>1</v>
-      </c>
-      <c r="G63" s="3">
-        <v>0</v>
-      </c>
-      <c r="H63" s="3">
-        <v>0</v>
-      </c>
-      <c r="I63" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J63" s="2" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A64" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64" t="b">
+        <v>1</v>
+      </c>
+      <c r="D64" t="b">
+        <v>1</v>
+      </c>
+      <c r="E64" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" t="b">
+        <v>1</v>
+      </c>
+      <c r="G64" s="3">
+        <v>0</v>
+      </c>
+      <c r="H64" s="3">
+        <v>0</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J64" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C64" t="b">
-        <v>1</v>
-      </c>
-      <c r="D64" t="b">
-        <v>1</v>
-      </c>
-      <c r="E64" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64" t="b">
-        <v>1</v>
-      </c>
-      <c r="G64" s="3">
-        <v>0</v>
-      </c>
-      <c r="H64" s="3">
-        <v>0</v>
-      </c>
-      <c r="I64" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J64" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A65" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65" t="b">
+        <v>1</v>
+      </c>
+      <c r="D65" t="b">
+        <v>1</v>
+      </c>
+      <c r="E65" t="b">
+        <v>1</v>
+      </c>
+      <c r="F65" t="b">
+        <v>1</v>
+      </c>
+      <c r="G65" s="3">
+        <v>0</v>
+      </c>
+      <c r="H65" s="3">
+        <v>0</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J65" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C65" t="b">
-        <v>1</v>
-      </c>
-      <c r="D65" t="b">
-        <v>1</v>
-      </c>
-      <c r="E65" t="b">
-        <v>1</v>
-      </c>
-      <c r="F65" t="b">
-        <v>1</v>
-      </c>
-      <c r="G65" s="3">
-        <v>0</v>
-      </c>
-      <c r="H65" s="3">
-        <v>0</v>
-      </c>
-      <c r="I65" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J65" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A66" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66" t="b">
+        <v>1</v>
+      </c>
+      <c r="D66" t="b">
+        <v>1</v>
+      </c>
+      <c r="E66" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" t="b">
+        <v>1</v>
+      </c>
+      <c r="G66" s="3">
+        <v>0</v>
+      </c>
+      <c r="H66" s="3">
+        <v>0</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J66" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C66" t="b">
-        <v>1</v>
-      </c>
-      <c r="D66" t="b">
-        <v>1</v>
-      </c>
-      <c r="E66" t="b">
-        <v>1</v>
-      </c>
-      <c r="F66" t="b">
-        <v>1</v>
-      </c>
-      <c r="G66" s="3">
-        <v>0</v>
-      </c>
-      <c r="H66" s="3">
-        <v>0</v>
-      </c>
-      <c r="I66" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J66" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A67" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67" t="b">
+        <v>1</v>
+      </c>
+      <c r="D67" t="b">
+        <v>1</v>
+      </c>
+      <c r="E67" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" t="b">
+        <v>1</v>
+      </c>
+      <c r="G67" s="3">
+        <v>0</v>
+      </c>
+      <c r="H67" s="3">
+        <v>0</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J67" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C67" t="b">
-        <v>1</v>
-      </c>
-      <c r="D67" t="b">
-        <v>1</v>
-      </c>
-      <c r="E67" t="b">
-        <v>1</v>
-      </c>
-      <c r="F67" t="b">
-        <v>1</v>
-      </c>
-      <c r="G67" s="3">
-        <v>0</v>
-      </c>
-      <c r="H67" s="3">
-        <v>0</v>
-      </c>
-      <c r="I67" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J67" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="C68" t="b">
         <v>1</v>
       </c>
@@ -3825,16 +3826,16 @@
         <v>0</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J68" s="1"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C69" t="b">
         <v>1</v>
@@ -3852,16 +3853,16 @@
         <v>0</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J69" s="1"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C70" t="b">
         <v>1</v>
@@ -3879,16 +3880,16 @@
         <v>0</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J70" s="1"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C71" t="b">
         <v>1</v>
@@ -3906,16 +3907,16 @@
         <v>0</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J71" s="1"/>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C72" t="b">
         <v>1</v>
@@ -3933,16 +3934,16 @@
         <v>0</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J72" s="1"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C73" t="b">
         <v>1</v>
@@ -3960,16 +3961,16 @@
         <v>0</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J73" s="1"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C74" t="b">
         <v>1</v>
@@ -3987,16 +3988,16 @@
         <v>0</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J74" s="1"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C75" t="b">
         <v>1</v>
@@ -4014,7 +4015,7 @@
         <v>0</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -4050,10 +4051,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" t="s">
         <v>151</v>
-      </c>
-      <c r="C1" t="s">
-        <v>152</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -4080,18 +4081,18 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="M1" t="s">
+        <v>199</v>
+      </c>
+      <c r="N1" t="s">
         <v>200</v>
-      </c>
-      <c r="N1" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -4118,19 +4119,19 @@
         <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -4175,13 +4176,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" t="s">
         <v>192</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>193</v>
-      </c>
-      <c r="C1" t="s">
-        <v>194</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
@@ -4189,16 +4190,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="C2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -4222,7 +4223,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4244,10 +4245,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" t="s">
         <v>151</v>
-      </c>
-      <c r="C1" t="s">
-        <v>152</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -4274,21 +4275,21 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
+        <v>152</v>
+      </c>
+      <c r="M1" t="s">
         <v>153</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>154</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>155</v>
-      </c>
-      <c r="O1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B2">
         <v>11</v>
@@ -4315,20 +4316,20 @@
         <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4392,10 +4393,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" t="s">
         <v>151</v>
-      </c>
-      <c r="C1" t="s">
-        <v>152</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -4422,81 +4423,81 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" t="s">
         <v>97</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>98</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>99</v>
       </c>
-      <c r="O1" t="s">
-        <v>100</v>
-      </c>
       <c r="P1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="R1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="S1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="U1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="W1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="X1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Y1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Z1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AA1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AB1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AC1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AD1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AE1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AG1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AH1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AI1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B2">
         <v>15</v>
@@ -4523,82 +4524,82 @@
         <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="W2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Y2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Z2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AB2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AC2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AD2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AE2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AF2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AG2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AH2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AI2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -4653,10 +4654,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" t="s">
         <v>151</v>
-      </c>
-      <c r="C1" t="s">
-        <v>152</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -4683,63 +4684,63 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
+        <v>159</v>
+      </c>
+      <c r="M1" t="s">
+        <v>152</v>
+      </c>
+      <c r="N1" t="s">
         <v>160</v>
       </c>
-      <c r="M1" t="s">
-        <v>153</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>161</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>162</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>163</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>164</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>165</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>166</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>167</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>168</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>169</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>170</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z1" t="s">
         <v>171</v>
       </c>
-      <c r="Y1" t="s">
-        <v>156</v>
-      </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>172</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>173</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>174</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B2">
         <v>211</v>
@@ -4766,64 +4767,64 @@
         <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="T2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="U2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="X2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Z2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AA2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AB2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AC2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4849,8 +4850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4873,10 +4874,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" t="s">
         <v>151</v>
-      </c>
-      <c r="C1" t="s">
-        <v>152</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -4903,24 +4904,24 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M1" t="s">
+        <v>214</v>
+      </c>
+      <c r="N1" t="s">
         <v>215</v>
-      </c>
-      <c r="N1" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2">
         <v>128</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -4941,19 +4942,19 @@
         <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="M2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -5006,10 +5007,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" t="s">
         <v>151</v>
-      </c>
-      <c r="C1" t="s">
-        <v>152</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -5036,21 +5037,21 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
+        <v>204</v>
+      </c>
+      <c r="M1" t="s">
         <v>205</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>206</v>
       </c>
-      <c r="N1" t="s">
-        <v>207</v>
-      </c>
       <c r="O1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B2">
         <v>256</v>
@@ -5077,22 +5078,22 @@
         <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -5143,10 +5144,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" t="s">
         <v>151</v>
-      </c>
-      <c r="C1" t="s">
-        <v>152</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -5173,21 +5174,21 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
+        <v>177</v>
+      </c>
+      <c r="M1" t="s">
         <v>178</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>179</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>180</v>
-      </c>
-      <c r="O1" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B2">
         <v>32</v>
@@ -5214,20 +5215,20 @@
         <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -5254,7 +5255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -5278,10 +5279,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" t="s">
         <v>151</v>
-      </c>
-      <c r="C1" t="s">
-        <v>152</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -5308,21 +5309,21 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
+        <v>182</v>
+      </c>
+      <c r="M1" t="s">
         <v>183</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>184</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>185</v>
-      </c>
-      <c r="O1" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -5349,22 +5350,22 @@
         <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -5413,10 +5414,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" t="s">
         <v>151</v>
-      </c>
-      <c r="C1" t="s">
-        <v>152</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -5443,15 +5444,15 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B2">
         <v>512</v>
@@ -5478,16 +5479,16 @@
         <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed for property radio description
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvsheng.huang\Desktop\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Struct\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="19560" windowHeight="8460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Property" sheetId="1" r:id="rId1"/>
@@ -32,7 +37,7 @@
     <author>pengbo.yang</author>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -41,11 +46,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">物品配置ID</t>
+          <t>物品配置ID</t>
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -54,11 +59,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">强化等级</t>
+          <t>强化等级</t>
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -67,11 +72,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">镶嵌宝石，逗号分隔</t>
+          <t>镶嵌宝石，逗号分隔</t>
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -80,7 +85,7 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">附魔等级</t>
+          <t>附魔等级</t>
         </r>
       </text>
     </comment>
@@ -94,7 +99,7 @@
     <author>pengbo.yang</author>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -103,11 +108,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">物品配置ID</t>
+          <t>物品配置ID</t>
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -116,11 +121,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">强化等级</t>
+          <t>强化等级</t>
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -129,11 +134,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">镶嵌宝石，逗号分隔</t>
+          <t>镶嵌宝石，逗号分隔</t>
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -142,11 +147,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">附魔等级</t>
+          <t>附魔等级</t>
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="P1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -155,11 +160,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">物品配置ID</t>
+          <t>物品配置ID</t>
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0">
+    <comment ref="Q1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -168,11 +173,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">强化等级</t>
+          <t>强化等级</t>
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0">
+    <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -181,11 +186,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">镶嵌宝石，逗号分隔</t>
+          <t>镶嵌宝石，逗号分隔</t>
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0">
+    <comment ref="S1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -194,7 +199,7 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">附魔等级</t>
+          <t>附魔等级</t>
         </r>
       </text>
     </comment>
@@ -206,10 +211,9 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>pengbo.yang</author>
-    <author>杨鹏博</author>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -218,11 +222,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">关卡ID</t>
+          <t>关卡ID</t>
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -236,7 +240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -245,7 +249,7 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">通过时的星级</t>
+          <t>通过时的星级</t>
         </r>
       </text>
     </comment>
@@ -257,10 +261,9 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>pengbo.yang</author>
-    <author>杨鹏博</author>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -269,11 +272,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">怪物GUID</t>
+          <t>怪物GUID</t>
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -282,11 +285,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">掉落道具ID</t>
+          <t>掉落道具ID</t>
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -295,11 +298,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">掉落道具数量</t>
+          <t>掉落道具数量</t>
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -308,7 +311,7 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">领取状态：
+          <t>领取状态：
 0 初始状态
 1 可以领
 2 领过了</t>
@@ -325,7 +328,7 @@
     <author>pengbo.yang</author>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -334,11 +337,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">物品配置ID</t>
+          <t>物品配置ID</t>
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -347,11 +350,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">强化等级</t>
+          <t>强化等级</t>
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -360,11 +363,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">镶嵌宝石，逗号分隔</t>
+          <t>镶嵌宝石，逗号分隔</t>
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -373,7 +376,7 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">附魔等级</t>
+          <t>附魔等级</t>
         </r>
       </text>
     </comment>
@@ -387,7 +390,7 @@
     <author>pengbo.yang</author>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -396,11 +399,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">物品配置ID</t>
+          <t>物品配置ID</t>
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -409,11 +412,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">强化等级</t>
+          <t>强化等级</t>
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -422,11 +425,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">镶嵌宝石，逗号分隔</t>
+          <t>镶嵌宝石，逗号分隔</t>
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -435,7 +438,7 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">附魔等级</t>
+          <t>附魔等级</t>
         </r>
       </text>
     </comment>
@@ -447,10 +450,9 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>pengbo.yang</author>
-    <author>杨鹏博</author>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -459,11 +461,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">任务ID</t>
+          <t>任务ID</t>
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -472,11 +474,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">任务状态，见NFDefine.proto中ETaskState</t>
+          <t>任务状态，见NFDefine.proto中ETaskState</t>
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -485,7 +487,7 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">当前进度</t>
+          <t>当前进度</t>
         </r>
       </text>
     </comment>
@@ -499,7 +501,7 @@
     <author>pengbo.yang</author>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -508,11 +510,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">物品配置ID</t>
+          <t>物品配置ID</t>
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -521,7 +523,7 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">强化等级</t>
+          <t>强化等级</t>
         </r>
       </text>
     </comment>
@@ -530,7 +532,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="215">
   <si>
     <t>Id</t>
   </si>
@@ -1180,14 +1182,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1207,7 +1203,13 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -1235,23 +1237,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1272,14 +1259,19 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
-    <cellStyle name="百分比" xfId="4" builtinId="5"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1578,6 +1570,7 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -1610,15 +1603,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="J82" sqref="J82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="23.875" customWidth="1"/>
     <col min="2" max="2" width="8.25" customWidth="1"/>
@@ -1631,7 +1623,7 @@
     <col min="10" max="10" width="81" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1663,7 +1655,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1695,7 +1687,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1727,7 +1719,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -1759,7 +1751,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -1791,7 +1783,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -1823,7 +1815,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -1855,7 +1847,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -1887,7 +1879,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -1919,7 +1911,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
@@ -1951,7 +1943,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
@@ -1983,7 +1975,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
@@ -2015,7 +2007,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -2047,7 +2039,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
@@ -2079,7 +2071,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
@@ -2111,7 +2103,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>42</v>
       </c>
@@ -2143,7 +2135,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>44</v>
       </c>
@@ -2175,7 +2167,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>46</v>
       </c>
@@ -2207,7 +2199,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>48</v>
       </c>
@@ -2239,7 +2231,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>50</v>
       </c>
@@ -2271,7 +2263,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>52</v>
       </c>
@@ -2303,7 +2295,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>54</v>
       </c>
@@ -2335,7 +2327,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>56</v>
       </c>
@@ -2367,7 +2359,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>58</v>
       </c>
@@ -2399,7 +2391,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>60</v>
       </c>
@@ -2431,7 +2423,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>62</v>
       </c>
@@ -2463,7 +2455,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>64</v>
       </c>
@@ -2495,7 +2487,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>66</v>
       </c>
@@ -2527,7 +2519,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>68</v>
       </c>
@@ -2559,7 +2551,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>70</v>
       </c>
@@ -2591,7 +2583,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
@@ -2623,7 +2615,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>74</v>
       </c>
@@ -2655,7 +2647,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>76</v>
       </c>
@@ -2687,7 +2679,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>78</v>
       </c>
@@ -2719,7 +2711,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>80</v>
       </c>
@@ -2751,7 +2743,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>82</v>
       </c>
@@ -2783,7 +2775,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>84</v>
       </c>
@@ -2815,7 +2807,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>86</v>
       </c>
@@ -2847,7 +2839,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>88</v>
       </c>
@@ -2879,7 +2871,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>90</v>
       </c>
@@ -2911,7 +2903,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>92</v>
       </c>
@@ -2943,7 +2935,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>94</v>
       </c>
@@ -2975,7 +2967,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>96</v>
       </c>
@@ -3005,7 +2997,7 @@
       </c>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A44" s="3" t="s">
         <v>97</v>
       </c>
@@ -3037,7 +3029,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A45" s="3" t="s">
         <v>98</v>
       </c>
@@ -3069,7 +3061,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A46" s="3" t="s">
         <v>99</v>
       </c>
@@ -3101,7 +3093,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A47" s="3" t="s">
         <v>100</v>
       </c>
@@ -3133,7 +3125,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
         <v>102</v>
       </c>
@@ -3165,7 +3157,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A49" s="3" t="s">
         <v>104</v>
       </c>
@@ -3197,7 +3189,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A50" s="3" t="s">
         <v>106</v>
       </c>
@@ -3229,7 +3221,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A51" s="3" t="s">
         <v>108</v>
       </c>
@@ -3261,7 +3253,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A52" s="3" t="s">
         <v>110</v>
       </c>
@@ -3293,7 +3285,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A53" s="3" t="s">
         <v>112</v>
       </c>
@@ -3325,7 +3317,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A54" s="3" t="s">
         <v>114</v>
       </c>
@@ -3357,7 +3349,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A55" s="3" t="s">
         <v>116</v>
       </c>
@@ -3389,7 +3381,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A56" s="3" t="s">
         <v>118</v>
       </c>
@@ -3421,7 +3413,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A57" s="3" t="s">
         <v>120</v>
       </c>
@@ -3453,7 +3445,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A58" s="3" t="s">
         <v>122</v>
       </c>
@@ -3485,7 +3477,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A59" s="3" t="s">
         <v>124</v>
       </c>
@@ -3517,7 +3509,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A60" s="3" t="s">
         <v>126</v>
       </c>
@@ -3549,7 +3541,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A61" s="3" t="s">
         <v>128</v>
       </c>
@@ -3581,7 +3573,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A62" s="3" t="s">
         <v>130</v>
       </c>
@@ -3613,7 +3605,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A63" s="3" t="s">
         <v>132</v>
       </c>
@@ -3645,7 +3637,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A64" s="3" t="s">
         <v>134</v>
       </c>
@@ -3677,7 +3669,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A65" s="3" t="s">
         <v>136</v>
       </c>
@@ -3709,7 +3701,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A66" s="3" t="s">
         <v>138</v>
       </c>
@@ -3741,7 +3733,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A67" s="3" t="s">
         <v>140</v>
       </c>
@@ -3773,7 +3765,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
         <v>142</v>
       </c>
@@ -3800,7 +3792,7 @@
       </c>
       <c r="J68" s="1"/>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
         <v>144</v>
       </c>
@@ -3827,7 +3819,7 @@
       </c>
       <c r="J69" s="1"/>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
         <v>145</v>
       </c>
@@ -3854,7 +3846,7 @@
       </c>
       <c r="J70" s="1"/>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
         <v>146</v>
       </c>
@@ -3881,7 +3873,7 @@
       </c>
       <c r="J71" s="1"/>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
         <v>147</v>
       </c>
@@ -3908,7 +3900,7 @@
       </c>
       <c r="J72" s="1"/>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
         <v>148</v>
       </c>
@@ -3935,7 +3927,7 @@
       </c>
       <c r="J73" s="1"/>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
         <v>149</v>
       </c>
@@ -3962,7 +3954,7 @@
       </c>
       <c r="J74" s="1"/>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
         <v>150</v>
       </c>
@@ -3970,13 +3962,13 @@
         <v>15</v>
       </c>
       <c r="C75" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D75" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E75" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G75">
         <v>0</v>
@@ -3988,7 +3980,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A76" s="3" t="s">
         <v>151</v>
       </c>
@@ -4020,7 +4012,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A77" s="3" t="s">
         <v>153</v>
       </c>
@@ -4052,7 +4044,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
         <v>155</v>
       </c>
@@ -4085,34 +4077,34 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="7" max="7" width="10" customWidth="1"/>
     <col min="10" max="10" width="18.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4156,7 +4148,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>209</v>
       </c>
@@ -4201,6 +4193,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="6">
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="L1 M1"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:F2">
@@ -4219,30 +4212,28 @@
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.25" customWidth="1"/>
     <col min="2" max="2" width="12.75" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4256,7 +4247,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>212</v>
       </c>
@@ -4271,6 +4262,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
       <formula1>"TRUE,FALSE"</formula1>
@@ -4279,22 +4271,21 @@
       <formula1>"lua,python,C#,js"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.125" customWidth="1"/>
     <col min="2" max="3" width="7.125" customWidth="1"/>
@@ -4308,7 +4299,7 @@
     <col min="15" max="15" width="20.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4355,7 +4346,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>163</v>
       </c>
@@ -4401,31 +4392,31 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D1:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1048576">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="19.375" customWidth="1"/>
     <col min="2" max="3" width="7.125" customWidth="1"/>
@@ -4456,7 +4447,7 @@
     <col min="33" max="33" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4563,7 +4554,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>164</v>
       </c>
@@ -4671,34 +4662,34 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D1:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L$1:AI$1048576">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L1:AI1048576">
       <formula1>"int,string,float,object"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.75" customWidth="1"/>
     <col min="2" max="3" width="7.125" customWidth="1"/>
@@ -4717,7 +4708,7 @@
     <col min="29" max="29" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4806,7 +4797,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>182</v>
       </c>
@@ -4896,33 +4887,33 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D1:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L$1:AC$1048576">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L1:AC1048576">
       <formula1>"int,string,float,object"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.125" customWidth="1"/>
     <col min="2" max="3" width="7.125" customWidth="1"/>
@@ -4937,7 +4928,7 @@
     <col min="14" max="14" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4981,7 +4972,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>187</v>
       </c>
@@ -5026,35 +5017,35 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D$1:F$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G42">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="L$1:M$1048576"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="L1:M1048576"/>
   </dataValidations>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.125" customWidth="1"/>
     <col min="2" max="3" width="7.125" customWidth="1"/>
@@ -5070,7 +5061,7 @@
     <col min="15" max="15" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5117,7 +5108,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>192</v>
       </c>
@@ -5165,35 +5156,35 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D$1:F$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G42">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="L$1:M$1048576"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="L1:M1048576"/>
   </dataValidations>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.125" customWidth="1"/>
     <col min="2" max="3" width="7.125" customWidth="1"/>
@@ -5207,7 +5198,7 @@
     <col min="15" max="15" width="20.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5254,7 +5245,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>198</v>
       </c>
@@ -5300,34 +5291,34 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D1:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L$1:O$1048576">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L1:O1048576">
       <formula1>"int,float,string,object"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.125" customWidth="1"/>
     <col min="2" max="3" width="7.125" customWidth="1"/>
@@ -5342,7 +5333,7 @@
     <col min="15" max="15" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5389,7 +5380,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>202</v>
       </c>
@@ -5437,34 +5428,34 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D1:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L$1:O$1048576">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L1:O1048576">
       <formula1>"int,float,string,object"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.125" customWidth="1"/>
     <col min="2" max="3" width="7.125" customWidth="1"/>
@@ -5477,7 +5468,7 @@
     <col min="13" max="13" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5521,7 +5512,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>206</v>
       </c>
@@ -5566,23 +5557,24 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D$1:F$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G42">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L$1:M$1048576">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L1:M1048576">
       <formula1>"int,float,string,object"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix the merge error
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvsheng.huang\Desktop\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Struct\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\NoahGameFrame\_Out\Server\NFDataCfg\Excel_Struct\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -532,7 +532,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="216">
   <si>
     <t>Id</t>
   </si>
@@ -1177,6 +1177,10 @@
   </si>
   <si>
     <t>测试组件</t>
+  </si>
+  <si>
+    <t>View</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1606,8 +1610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="J82" sqref="J82"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1640,7 +1644,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>215</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
@@ -3781,6 +3785,9 @@
       <c r="E68" t="b">
         <v>1</v>
       </c>
+      <c r="F68" t="b">
+        <v>1</v>
+      </c>
       <c r="G68">
         <v>0</v>
       </c>
@@ -3808,6 +3815,9 @@
       <c r="E69" t="b">
         <v>1</v>
       </c>
+      <c r="F69" t="b">
+        <v>1</v>
+      </c>
       <c r="G69">
         <v>0</v>
       </c>
@@ -3835,6 +3845,9 @@
       <c r="E70" t="b">
         <v>1</v>
       </c>
+      <c r="F70" t="b">
+        <v>1</v>
+      </c>
       <c r="G70">
         <v>0</v>
       </c>
@@ -3862,6 +3875,9 @@
       <c r="E71" t="b">
         <v>1</v>
       </c>
+      <c r="F71" t="b">
+        <v>1</v>
+      </c>
       <c r="G71">
         <v>0</v>
       </c>
@@ -3889,6 +3905,9 @@
       <c r="E72" t="b">
         <v>1</v>
       </c>
+      <c r="F72" t="b">
+        <v>1</v>
+      </c>
       <c r="G72">
         <v>0</v>
       </c>
@@ -3916,6 +3935,9 @@
       <c r="E73" t="b">
         <v>1</v>
       </c>
+      <c r="F73" t="b">
+        <v>1</v>
+      </c>
       <c r="G73">
         <v>0</v>
       </c>
@@ -3943,6 +3965,9 @@
       <c r="E74" t="b">
         <v>1</v>
       </c>
+      <c r="F74" t="b">
+        <v>1</v>
+      </c>
       <c r="G74">
         <v>0</v>
       </c>
@@ -3970,6 +3995,9 @@
       <c r="E75" t="b">
         <v>0</v>
       </c>
+      <c r="F75" t="b">
+        <v>1</v>
+      </c>
       <c r="G75">
         <v>0</v>
       </c>
@@ -3991,13 +4019,13 @@
         <v>0</v>
       </c>
       <c r="D76" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E76" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F76" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G76" s="4">
         <v>0</v>
@@ -4023,13 +4051,13 @@
         <v>0</v>
       </c>
       <c r="D77" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E77" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F77" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G77" s="4">
         <v>0</v>
@@ -4052,7 +4080,7 @@
         <v>30</v>
       </c>
       <c r="C78" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D78" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
modify queue lock, modify the way of saving player'data
Former-commit-id: a4f0f5b43a0f24e4747ed082a4c0f3d211df0eaa [formerly 9a3a3f7275fa1400d2b63b6d637072882bafc008]
Former-commit-id: 7db78d5f38def1345153e67ebd999a32362a5f2f
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
@@ -1640,7 +1640,7 @@
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+      <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3044,7 +3044,7 @@
         <v>1</v>
       </c>
       <c r="E44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" t="b">
         <v>1</v>
@@ -3076,7 +3076,7 @@
         <v>1</v>
       </c>
       <c r="E45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45" t="b">
         <v>1</v>
@@ -3108,7 +3108,7 @@
         <v>1</v>
       </c>
       <c r="E46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46" t="b">
         <v>1</v>
@@ -3140,7 +3140,7 @@
         <v>1</v>
       </c>
       <c r="E47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F47" t="b">
         <v>1</v>
@@ -3172,7 +3172,7 @@
         <v>1</v>
       </c>
       <c r="E48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48" t="b">
         <v>1</v>
@@ -3204,7 +3204,7 @@
         <v>1</v>
       </c>
       <c r="E49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49" t="b">
         <v>1</v>
@@ -3236,7 +3236,7 @@
         <v>1</v>
       </c>
       <c r="E50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F50" t="b">
         <v>1</v>
@@ -3268,7 +3268,7 @@
         <v>1</v>
       </c>
       <c r="E51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F51" t="b">
         <v>1</v>
@@ -3300,7 +3300,7 @@
         <v>1</v>
       </c>
       <c r="E52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F52" t="b">
         <v>1</v>
@@ -3332,7 +3332,7 @@
         <v>1</v>
       </c>
       <c r="E53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F53" t="b">
         <v>1</v>
@@ -3364,7 +3364,7 @@
         <v>1</v>
       </c>
       <c r="E54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F54" t="b">
         <v>1</v>
@@ -3396,7 +3396,7 @@
         <v>1</v>
       </c>
       <c r="E55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F55" t="b">
         <v>1</v>
@@ -3428,7 +3428,7 @@
         <v>1</v>
       </c>
       <c r="E56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F56" t="b">
         <v>1</v>
@@ -3460,7 +3460,7 @@
         <v>1</v>
       </c>
       <c r="E57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F57" t="b">
         <v>1</v>
@@ -3492,7 +3492,7 @@
         <v>1</v>
       </c>
       <c r="E58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F58" t="b">
         <v>1</v>
@@ -3524,7 +3524,7 @@
         <v>1</v>
       </c>
       <c r="E59" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F59" t="b">
         <v>1</v>
@@ -3556,7 +3556,7 @@
         <v>1</v>
       </c>
       <c r="E60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F60" t="b">
         <v>1</v>
@@ -3588,7 +3588,7 @@
         <v>1</v>
       </c>
       <c r="E61" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F61" t="b">
         <v>1</v>
@@ -3620,7 +3620,7 @@
         <v>1</v>
       </c>
       <c r="E62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F62" t="b">
         <v>1</v>
@@ -3652,7 +3652,7 @@
         <v>1</v>
       </c>
       <c r="E63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F63" t="b">
         <v>1</v>
@@ -3684,7 +3684,7 @@
         <v>1</v>
       </c>
       <c r="E64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F64" t="b">
         <v>1</v>
@@ -3716,7 +3716,7 @@
         <v>1</v>
       </c>
       <c r="E65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F65" t="b">
         <v>1</v>
@@ -3748,7 +3748,7 @@
         <v>1</v>
       </c>
       <c r="E66" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F66" t="b">
         <v>1</v>
@@ -3780,7 +3780,7 @@
         <v>1</v>
       </c>
       <c r="E67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F67" t="b">
         <v>1</v>
@@ -4038,10 +4038,10 @@
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" t="s">
         <v>15</v>
       </c>
       <c r="C76" t="b">
@@ -4056,24 +4056,24 @@
       <c r="F76" t="b">
         <v>1</v>
       </c>
-      <c r="G76" s="4">
-        <v>0</v>
-      </c>
-      <c r="H76" s="4">
-        <v>0</v>
-      </c>
-      <c r="I76" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J76" s="3" t="s">
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+      <c r="I76" t="s">
+        <v>12</v>
+      </c>
+      <c r="J76" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A77" s="3" t="s">
+      <c r="A77" t="s">
         <v>152</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" t="s">
         <v>15</v>
       </c>
       <c r="C77" t="b">
@@ -4088,16 +4088,16 @@
       <c r="F77" t="b">
         <v>1</v>
       </c>
-      <c r="G77" s="4">
-        <v>0</v>
-      </c>
-      <c r="H77" s="4">
-        <v>0</v>
-      </c>
-      <c r="I77" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J77" s="3" t="s">
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77" t="s">
+        <v>12</v>
+      </c>
+      <c r="J77" t="s">
         <v>153</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modified property for player
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
@@ -9,23 +9,27 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8460" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Property" sheetId="1" r:id="rId1"/>
     <sheet name="Record_PlayerViewItem" sheetId="2" r:id="rId2"/>
-    <sheet name="Record_CommPropertyValue" sheetId="3" r:id="rId3"/>
-    <sheet name="Record_BagItemList" sheetId="4" r:id="rId4"/>
-    <sheet name="Record_EctypeList" sheetId="5" r:id="rId5"/>
-    <sheet name="Record_DropItemList" sheetId="6" r:id="rId6"/>
-    <sheet name="Record_SkillTable" sheetId="7" r:id="rId7"/>
-    <sheet name="Record_TaskMonsterList" sheetId="8" r:id="rId8"/>
-    <sheet name="Record_TaskList" sheetId="9" r:id="rId9"/>
-    <sheet name="Record_PvpList" sheetId="10" r:id="rId10"/>
-    <sheet name="Record_ChatGroup" sheetId="12" r:id="rId11"/>
-    <sheet name="Component" sheetId="11" r:id="rId12"/>
+    <sheet name="Record_PlayerHero" sheetId="15" r:id="rId3"/>
+    <sheet name="Record_BagEquipList" sheetId="13" r:id="rId4"/>
+    <sheet name="Record_BagItemList" sheetId="4" r:id="rId5"/>
+    <sheet name="Record_CommPropertyValue" sheetId="3" r:id="rId6"/>
+    <sheet name="Record_EctypeList" sheetId="5" r:id="rId7"/>
+    <sheet name="Record_DropItemList" sheetId="6" r:id="rId8"/>
+    <sheet name="Record_SkillTable" sheetId="7" r:id="rId9"/>
+    <sheet name="Record_TaskMonsterList" sheetId="8" r:id="rId10"/>
+    <sheet name="Record_TaskList" sheetId="9" r:id="rId11"/>
+    <sheet name="Record_PvpList" sheetId="10" r:id="rId12"/>
+    <sheet name="Record_ChatGroup" sheetId="12" r:id="rId13"/>
+    <sheet name="Component" sheetId="11" r:id="rId14"/>
   </sheets>
   <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="3" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="2" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
@@ -45,6 +49,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>物品配置ID</t>
@@ -58,6 +63,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>强化等级</t>
@@ -71,6 +77,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>镶嵌宝石，逗号分隔</t>
@@ -84,9 +91,48 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>附魔等级</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>pengbo.yang</author>
+  </authors>
+  <commentList>
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>聊天类型</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>聊天组的ID</t>
         </r>
       </text>
     </comment>
@@ -100,19 +146,6 @@
     <author>pengbo.yang</author>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>物品配置ID</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
@@ -120,9 +153,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>强化等级</t>
+          <t>物品配置ID</t>
         </r>
       </text>
     </comment>
@@ -133,9 +167,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>镶嵌宝石，逗号分隔</t>
+          <t>强化等级</t>
         </r>
       </text>
     </comment>
@@ -146,61 +181,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>附魔等级</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>物品配置ID</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Q1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>强化等级</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="R1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>镶嵌宝石，逗号分隔</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="S1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>附魔等级</t>
         </r>
       </text>
     </comment>
@@ -221,9 +205,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>关卡ID</t>
+          <t>物品配置ID</t>
         </r>
       </text>
     </comment>
@@ -234,10 +219,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">是否通关
-</t>
+          <t>强化等级</t>
         </r>
       </text>
     </comment>
@@ -248,9 +233,80 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>通过时的星级</t>
+          <t>镶嵌宝石，逗号分隔</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>附魔等级</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>物品配置ID</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>强化等级</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>镶嵌宝石，逗号分隔</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>附魔等级</t>
         </r>
       </text>
     </comment>
@@ -271,9 +327,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>怪物GUID</t>
+          <t>关卡ID</t>
         </r>
       </text>
     </comment>
@@ -284,9 +341,11 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>掉落道具ID</t>
+          <t xml:space="preserve">是否通关
+</t>
         </r>
       </text>
     </comment>
@@ -297,25 +356,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>掉落道具数量</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>领取状态：
-0 初始状态
-1 可以领
-2 领过了</t>
+          <t>通过时的星级</t>
         </r>
       </text>
     </comment>
@@ -336,9 +380,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>物品配置ID</t>
+          <t>怪物GUID</t>
         </r>
       </text>
     </comment>
@@ -349,9 +394,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>强化等级</t>
+          <t>掉落道具ID</t>
         </r>
       </text>
     </comment>
@@ -362,9 +408,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>镶嵌宝石，逗号分隔</t>
+          <t>掉落道具数量</t>
         </r>
       </text>
     </comment>
@@ -375,9 +422,13 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>附魔等级</t>
+          <t>领取状态：
+0 初始状态
+1 可以领
+2 领过了</t>
         </r>
       </text>
     </comment>
@@ -398,6 +449,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>物品配置ID</t>
@@ -411,6 +463,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>强化等级</t>
@@ -424,6 +477,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>镶嵌宝石，逗号分隔</t>
@@ -437,6 +491,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>附魔等级</t>
@@ -460,9 +515,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>任务ID</t>
+          <t>物品配置ID</t>
         </r>
       </text>
     </comment>
@@ -473,9 +529,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>任务状态，见NFDefine.proto中ETaskState</t>
+          <t>强化等级</t>
         </r>
       </text>
     </comment>
@@ -486,9 +543,24 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>当前进度</t>
+          <t>镶嵌宝石，逗号分隔</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>附魔等级</t>
         </r>
       </text>
     </comment>
@@ -509,9 +581,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>物品配置ID</t>
+          <t>任务ID</t>
         </r>
       </text>
     </comment>
@@ -522,9 +595,24 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>强化等级</t>
+          <t>任务状态，见NFDefine.proto中ETaskState</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>当前进度</t>
         </r>
       </text>
     </comment>
@@ -545,9 +633,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>聊天类型</t>
+          <t>物品配置ID</t>
         </r>
       </text>
     </comment>
@@ -558,9 +647,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>聊天组的ID</t>
+          <t>强化等级</t>
         </r>
       </text>
     </comment>
@@ -569,7 +659,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="248">
   <si>
     <t>Id</t>
   </si>
@@ -1090,22 +1180,7 @@
     <t>InlayStone6</t>
   </si>
   <si>
-    <t>EnhancedLevel</t>
-  </si>
-  <si>
-    <t>SagecraftStone</t>
-  </si>
-  <si>
-    <t>RandProperty</t>
-  </si>
-  <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>BaseProperty</t>
-  </si>
-  <si>
-    <t>BagItemList</t>
   </si>
   <si>
     <t>普通背包</t>
@@ -1246,6 +1321,126 @@
   </si>
   <si>
     <t>VIP经验</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>BagEquipList</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>BagItemList</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>InlayStone7</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>InlayStone8</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>InlayStone10</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>InlayStone9</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>IntensifyLevel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>RandPropertyID</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ElementLevel1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ElementLevel2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ElementLevel3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ElementLevel4</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ElementLevel5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ElementLevel6</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ElementLevel7</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ElementLevel8</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ElementLevel9</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ElementLevel10</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>object</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>GUID</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exp</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>WearGUID</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Equip2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Equip1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Equip3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Equip4</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Equip5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Equip6</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlayerHero</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1253,7 +1448,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1264,23 +1459,27 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="10"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1292,6 +1491,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -1337,7 +1543,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1366,6 +1572,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1744,7 +1956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -1778,7 +1990,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
@@ -2211,7 +2423,7 @@
     </row>
     <row r="15" spans="1:10" s="7" customFormat="1">
       <c r="A15" s="6" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>15</v>
@@ -2243,34 +2455,34 @@
     </row>
     <row r="16" spans="1:10" s="9" customFormat="1">
       <c r="A16" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" s="9">
+        <v>0</v>
+      </c>
+      <c r="H16" s="9">
+        <v>0</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" s="8" t="s">
         <v>217</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G16" s="9">
-        <v>0</v>
-      </c>
-      <c r="H16" s="9">
-        <v>0</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="9" customFormat="1">
@@ -2403,7 +2615,7 @@
     </row>
     <row r="21" spans="1:10" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>15</v>
@@ -2430,7 +2642,7 @@
         <v>12</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="9" customFormat="1">
@@ -2462,7 +2674,7 @@
         <v>12</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="14.25" customHeight="1">
@@ -4208,7 +4420,7 @@
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B78" t="s">
         <v>15</v>
@@ -4318,6 +4530,275 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="16.125" customWidth="1"/>
+    <col min="2" max="3" width="7.125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="11.625" customWidth="1"/>
+    <col min="8" max="8" width="9.375" customWidth="1"/>
+    <col min="9" max="9" width="17.75" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="12.75" customWidth="1"/>
+    <col min="13" max="14" width="22.75" customWidth="1"/>
+    <col min="15" max="15" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>180</v>
+      </c>
+      <c r="M1" t="s">
+        <v>190</v>
+      </c>
+      <c r="N1" t="s">
+        <v>191</v>
+      </c>
+      <c r="O1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="L2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D1:F1048576">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L1:O1048576">
+      <formula1>"int,float,string,object"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="16.125" customWidth="1"/>
+    <col min="2" max="3" width="7.125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="11.625" customWidth="1"/>
+    <col min="8" max="8" width="9.375" customWidth="1"/>
+    <col min="9" max="9" width="17.75" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="12" max="12" width="12.75" customWidth="1"/>
+    <col min="13" max="13" width="17.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>192</v>
+      </c>
+      <c r="M1" t="s">
+        <v>195</v>
+      </c>
+      <c r="N1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2">
+        <v>512</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="L2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:F1048576">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G42">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L1:M1048576">
+      <formula1>"int,float,string,object"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4365,7 +4846,7 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="M1" t="s">
         <v>10</v>
@@ -4376,7 +4857,7 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -4406,7 +4887,7 @@
         <v>12</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="L2" t="s">
         <v>30</v>
@@ -4444,11 +4925,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
@@ -4489,15 +4970,15 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="M1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -4527,7 +5008,7 @@
         <v>12</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="L2" t="s">
         <v>15</v>
@@ -4558,12 +5039,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -4578,10 +5059,10 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
@@ -4589,16 +5070,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -4622,7 +5103,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -4750,10 +5231,607 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="16.125" customWidth="1"/>
+    <col min="2" max="3" width="7.125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="11.625" customWidth="1"/>
+    <col min="8" max="8" width="9.375" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="13" max="13" width="12.75" customWidth="1"/>
+    <col min="14" max="14" width="17.75" customWidth="1"/>
+    <col min="15" max="15" width="15.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>237</v>
+      </c>
+      <c r="M1" t="s">
+        <v>155</v>
+      </c>
+      <c r="N1" t="s">
+        <v>238</v>
+      </c>
+      <c r="O1" t="s">
+        <v>239</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="V1" s="10"/>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="M2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <dataValidations count="2">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D1:F1048576">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AN2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="12.75" customWidth="1"/>
+    <col min="2" max="3" width="7.125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="11.625" customWidth="1"/>
+    <col min="8" max="8" width="9.375" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="14" max="14" width="12.75" customWidth="1"/>
+    <col min="16" max="16" width="16.5" customWidth="1"/>
+    <col min="17" max="17" width="17.75" customWidth="1"/>
+    <col min="18" max="18" width="8.375" customWidth="1"/>
+    <col min="19" max="19" width="14" customWidth="1"/>
+    <col min="20" max="29" width="16.5" customWidth="1"/>
+    <col min="30" max="30" width="19" customWidth="1"/>
+    <col min="31" max="40" width="20.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:40">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>162</v>
+      </c>
+      <c r="M1" t="s">
+        <v>240</v>
+      </c>
+      <c r="N1" t="s">
+        <v>155</v>
+      </c>
+      <c r="O1" t="s">
+        <v>164</v>
+      </c>
+      <c r="P1" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>225</v>
+      </c>
+      <c r="R1" t="s">
+        <v>173</v>
+      </c>
+      <c r="S1" t="s">
+        <v>166</v>
+      </c>
+      <c r="T1" t="s">
+        <v>167</v>
+      </c>
+      <c r="U1" t="s">
+        <v>168</v>
+      </c>
+      <c r="V1" t="s">
+        <v>169</v>
+      </c>
+      <c r="W1" t="s">
+        <v>170</v>
+      </c>
+      <c r="X1" t="s">
+        <v>171</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>231</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>232</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>233</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>234</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40">
+      <c r="A2" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2">
+        <v>256</v>
+      </c>
+      <c r="C2">
+        <v>29</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="L2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S2" t="s">
+        <v>15</v>
+      </c>
+      <c r="T2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U2" t="s">
+        <v>11</v>
+      </c>
+      <c r="V2" t="s">
+        <v>11</v>
+      </c>
+      <c r="W2" t="s">
+        <v>11</v>
+      </c>
+      <c r="X2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <dataValidations count="4">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D1:F1048576">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="S2:S1048576 Z2:AN1048576 T1:Y1048576 R1:R1048576 L1:L1048576 N1:P1048576 M2:M1048576">
+      <formula1>"int,string,float,object"</formula1>
+    </dataValidation>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="S1 Q1:Q1048576 Z1:AN1 M1"/>
+  </dataValidations>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="12.75" customWidth="1"/>
+    <col min="2" max="3" width="7.125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="11.625" customWidth="1"/>
+    <col min="8" max="8" width="9.375" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="12" max="12" width="12.75" customWidth="1"/>
+    <col min="13" max="13" width="14" customWidth="1"/>
+    <col min="15" max="15" width="16.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>155</v>
+      </c>
+      <c r="M1" t="s">
+        <v>163</v>
+      </c>
+      <c r="N1" t="s">
+        <v>164</v>
+      </c>
+      <c r="O1" t="s">
+        <v>165</v>
+      </c>
+      <c r="P1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2">
+        <v>128</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="L2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D1:F1048576">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L1:P1048576">
+      <formula1>"int,string,float,object"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -4764,6 +5842,7 @@
     <col min="5" max="5" width="11.625" customWidth="1"/>
     <col min="8" max="8" width="9.375" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="26.875" customWidth="1"/>
     <col min="12" max="12" width="12.75" customWidth="1"/>
     <col min="13" max="13" width="17.75" customWidth="1"/>
     <col min="14" max="14" width="15.25" customWidth="1"/>
@@ -5021,231 +6100,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="12.75" customWidth="1"/>
-    <col min="2" max="3" width="7.125" customWidth="1"/>
-    <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="5" width="11.625" customWidth="1"/>
-    <col min="8" max="8" width="9.375" customWidth="1"/>
-    <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="13" max="13" width="12.75" customWidth="1"/>
-    <col min="14" max="14" width="14" customWidth="1"/>
-    <col min="16" max="16" width="16.5" customWidth="1"/>
-    <col min="17" max="17" width="14" customWidth="1"/>
-    <col min="18" max="23" width="16.5" customWidth="1"/>
-    <col min="24" max="24" width="19" customWidth="1"/>
-    <col min="25" max="26" width="20.25" customWidth="1"/>
-    <col min="27" max="27" width="17.75" customWidth="1"/>
-    <col min="29" max="29" width="17.75" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>162</v>
-      </c>
-      <c r="M1" t="s">
-        <v>155</v>
-      </c>
-      <c r="N1" t="s">
-        <v>163</v>
-      </c>
-      <c r="O1" t="s">
-        <v>164</v>
-      </c>
-      <c r="P1" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>166</v>
-      </c>
-      <c r="R1" t="s">
-        <v>167</v>
-      </c>
-      <c r="S1" t="s">
-        <v>168</v>
-      </c>
-      <c r="T1" t="s">
-        <v>169</v>
-      </c>
-      <c r="U1" t="s">
-        <v>170</v>
-      </c>
-      <c r="V1" t="s">
-        <v>171</v>
-      </c>
-      <c r="W1" t="s">
-        <v>172</v>
-      </c>
-      <c r="X1" t="s">
-        <v>173</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>158</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>174</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>175</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>176</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29">
-      <c r="A2" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B2">
-        <v>211</v>
-      </c>
-      <c r="C2">
-        <v>18</v>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="L2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" t="s">
-        <v>11</v>
-      </c>
-      <c r="S2" t="s">
-        <v>11</v>
-      </c>
-      <c r="T2" t="s">
-        <v>11</v>
-      </c>
-      <c r="U2" t="s">
-        <v>11</v>
-      </c>
-      <c r="V2" t="s">
-        <v>11</v>
-      </c>
-      <c r="W2" t="s">
-        <v>11</v>
-      </c>
-      <c r="X2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D1:F1048576">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1048576">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L1:AC1048576">
-      <formula1>"int,string,float,object"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -5303,18 +6158,18 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="M1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="N1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B2">
         <v>128</v>
@@ -5344,7 +6199,7 @@
         <v>12</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>15</v>
@@ -5377,7 +6232,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -5436,21 +6291,21 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="M1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="N1" t="s">
         <v>163</v>
       </c>
       <c r="O1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B2">
         <v>256</v>
@@ -5480,7 +6335,7 @@
         <v>12</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>30</v>
@@ -5516,7 +6371,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -5573,21 +6428,21 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="M1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="N1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="O1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B2">
         <v>32</v>
@@ -5648,273 +6503,4 @@
   <headerFooter alignWithMargins="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="16.125" customWidth="1"/>
-    <col min="2" max="3" width="7.125" customWidth="1"/>
-    <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="5" width="11.625" customWidth="1"/>
-    <col min="8" max="8" width="9.375" customWidth="1"/>
-    <col min="9" max="9" width="17.75" customWidth="1"/>
-    <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="12.75" customWidth="1"/>
-    <col min="13" max="14" width="22.75" customWidth="1"/>
-    <col min="15" max="15" width="10.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>185</v>
-      </c>
-      <c r="M1" t="s">
-        <v>195</v>
-      </c>
-      <c r="N1" t="s">
-        <v>196</v>
-      </c>
-      <c r="O1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B2">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="L2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D1:F1048576">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1048576">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L1:O1048576">
-      <formula1>"int,float,string,object"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="16.125" customWidth="1"/>
-    <col min="2" max="3" width="7.125" customWidth="1"/>
-    <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="5" width="11.625" customWidth="1"/>
-    <col min="8" max="8" width="9.375" customWidth="1"/>
-    <col min="9" max="9" width="17.75" customWidth="1"/>
-    <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="12" max="12" width="12.75" customWidth="1"/>
-    <col min="13" max="13" width="17.75" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>197</v>
-      </c>
-      <c r="M1" t="s">
-        <v>200</v>
-      </c>
-      <c r="N1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B2">
-        <v>512</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="L2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:F1048576">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G42">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1048576">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L1:M1048576">
-      <formula1>"int,float,string,object"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add Tile record and tile module functions
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NF\NoahGameFrame\_Out\Server\NFDataCfg\Excel_Struct\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\project\NFrame_CPP\_Out\Server\NFDataCfg\Excel_Struct\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19455" windowHeight="8985" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19455" windowHeight="8985" firstSheet="11" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Property" sheetId="1" r:id="rId1"/>
@@ -27,11 +27,13 @@
     <sheet name="Record_ChatGroup" sheetId="13" r:id="rId13"/>
     <sheet name="Record_BuildingList" sheetId="14" r:id="rId14"/>
     <sheet name="Record_BuildingProduce" sheetId="15" r:id="rId15"/>
-    <sheet name="Component" sheetId="16" r:id="rId16"/>
+    <sheet name="Record_TileList" sheetId="17" r:id="rId16"/>
+    <sheet name="Component" sheetId="16" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="3" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="2" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="15" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
@@ -175,6 +177,29 @@
             <charset val="134"/>
           </rPr>
           <t>建筑ID</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>pengbo.yang</author>
+  </authors>
+  <commentList>
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Tile编号</t>
         </r>
       </text>
     </comment>
@@ -683,7 +708,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="281">
   <si>
     <t>Id</t>
   </si>
@@ -1690,6 +1715,42 @@
       </rPr>
       <t>1</t>
     </r>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF006100"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ileList</t>
+    </r>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>TileID</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>TileType</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
@@ -1826,7 +1887,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1873,6 +1934,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -5661,6 +5725,144 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7.125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="11.625" customWidth="1"/>
+    <col min="8" max="8" width="9.375" customWidth="1"/>
+    <col min="9" max="9" width="17.125" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="12" max="12" width="12.75" customWidth="1"/>
+    <col min="13" max="13" width="13.875" customWidth="1"/>
+    <col min="15" max="15" width="11.625" customWidth="1"/>
+    <col min="16" max="16" width="13.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="B2" s="2">
+        <v>20480</v>
+      </c>
+      <c r="C2" s="2">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2">
+      <formula1>"int,float,string,object"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L2:L41 O2 M2">
+      <formula1>"int,float,string,object"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D1:F1048576">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="L1:M1 O1 L42:L1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1"/>
+  </dataValidations>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -5854,7 +6056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed bug for hero module
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="21495" windowHeight="10350" firstSheet="2" activeTab="2"/>
+    <workbookView windowWidth="27765" windowHeight="15450" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Property" sheetId="1" r:id="rId1"/>
@@ -477,7 +477,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214">
   <si>
     <t>Id</t>
   </si>
@@ -894,29 +894,6 @@
   </si>
   <si>
     <t>Equip6</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Equip</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>7</t>
-    </r>
-  </si>
-  <si>
-    <t>Equip8</t>
   </si>
   <si>
     <r>
@@ -1019,90 +996,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Talent</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>6</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Talent</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>7</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Talent</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>8</t>
-    </r>
-  </si>
-  <si>
-    <t>TalentLevel1</t>
-  </si>
-  <si>
-    <t>TalentLevel2</t>
-  </si>
-  <si>
-    <t>TalentLevel3</t>
-  </si>
-  <si>
-    <t>TalentLevel4</t>
-  </si>
-  <si>
-    <t>TalentLevel5</t>
-  </si>
-  <si>
-    <t>TalentLevel6</t>
-  </si>
-  <si>
-    <t>TalentLevel7</t>
-  </si>
-  <si>
-    <t>TalentLevel8</t>
-  </si>
-  <si>
     <t>Skill1</t>
   </si>
   <si>
@@ -1116,24 +1009,6 @@
   </si>
   <si>
     <t>Skill5</t>
-  </si>
-  <si>
-    <t>SkillLevel1</t>
-  </si>
-  <si>
-    <t>SkillLevel2</t>
-  </si>
-  <si>
-    <t>SkillLevel3</t>
-  </si>
-  <si>
-    <t>SkillLevel4</t>
-  </si>
-  <si>
-    <t>SkillLevel5</t>
-  </si>
-  <si>
-    <t>FightState</t>
   </si>
   <si>
     <t>FightSkill</t>
@@ -1336,10 +1211,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -1387,8 +1262,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1397,52 +1273,6 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1457,7 +1287,35 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1471,23 +1329,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1502,16 +1361,32 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1556,7 +1431,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1568,13 +1455,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1586,13 +1515,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1604,85 +1569,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1694,31 +1581,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1735,60 +1610,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1818,11 +1639,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1835,99 +1669,140 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1936,52 +1811,52 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4447,33 +4322,33 @@
         <v>9</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="5" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
       <c r="B2" s="2">
         <v>128</v>
@@ -4531,18 +4406,18 @@
   </sheetData>
   <dataValidations count="6">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2">
+      <formula1>"int,float,string,object"</formula1>
+    </dataValidation>
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="L1:M1 O1:Q1 L42:L1048576"/>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="M2 O2:Q2 L2:L41">
       <formula1>"int,float,string,object"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2">
-      <formula1>"int,float,string,object"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
+      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
       <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
-      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4610,33 +4485,33 @@
         <v>9</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="3" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="B2" s="2">
         <v>128</v>
@@ -4694,18 +4569,18 @@
   </sheetData>
   <dataValidations count="6">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2">
+      <formula1>"int,float,string,object"</formula1>
+    </dataValidation>
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="L1:M1 O1:Q1 L42:L1048576"/>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="M2 O2:Q2 L2:L41">
       <formula1>"int,float,string,object"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2">
-      <formula1>"int,float,string,object"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
+      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
       <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
-      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4735,10 +4610,10 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="C1" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
@@ -4746,25 +4621,25 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"lua,python,C#,js"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
       <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>"lua,python,C#,js"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4776,10 +4651,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AZ2"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -4793,14 +4668,10 @@
     <col min="13" max="13" width="12.75" customWidth="1"/>
     <col min="14" max="14" width="17.75" customWidth="1"/>
     <col min="15" max="16" width="15.25" customWidth="1"/>
-    <col min="33" max="40" width="13.75" customWidth="1"/>
-    <col min="46" max="46" width="11.625" customWidth="1"/>
-    <col min="50" max="50" width="12.75" customWidth="1"/>
-    <col min="51" max="51" width="22.75" customWidth="1"/>
-    <col min="52" max="52" width="9" customWidth="1"/>
+    <col min="33" max="33" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52">
+    <row r="1" spans="1:33">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4897,76 +4768,19 @@
       <c r="AF1" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="AG1" s="7" t="s">
+      <c r="AG1" t="s">
         <v>149</v>
       </c>
-      <c r="AH1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:33">
+      <c r="A2" s="6" t="s">
         <v>150</v>
-      </c>
-      <c r="AI1" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="AJ1" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="AK1" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="AL1" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="AM1" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="AN1" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="AO1" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="AP1" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="AQ1" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="AR1" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="AS1" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="AT1" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="AU1" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="AV1" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="AW1" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="AX1" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="AY1" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="2" spans="1:52">
-      <c r="A2" s="6" t="s">
-        <v>169</v>
       </c>
       <c r="B2">
         <v>64</v>
       </c>
       <c r="C2">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -5023,11 +4837,11 @@
       <c r="V2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="W2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>30</v>
+      <c r="W2" t="s">
+        <v>11</v>
+      </c>
+      <c r="X2" t="s">
+        <v>11</v>
       </c>
       <c r="Y2" t="s">
         <v>11</v>
@@ -5054,73 +4868,16 @@
         <v>11</v>
       </c>
       <c r="AG2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AZ2" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
       <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
-      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5135,7 +4892,7 @@
   <sheetPr/>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -5182,12 +4939,12 @@
         <v>129</v>
       </c>
       <c r="M1" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="6" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -5226,11 +4983,11 @@
     </row>
   </sheetData>
   <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2 D1:F2">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C2">
       <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2 D1:F2">
-      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -5303,93 +5060,93 @@
         <v>129</v>
       </c>
       <c r="M1" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="N1" t="s">
         <v>130</v>
       </c>
       <c r="O1" t="s">
+        <v>154</v>
+      </c>
+      <c r="P1" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>156</v>
+      </c>
+      <c r="R1" t="s">
+        <v>157</v>
+      </c>
+      <c r="S1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T1" t="s">
+        <v>159</v>
+      </c>
+      <c r="U1" t="s">
+        <v>160</v>
+      </c>
+      <c r="V1" t="s">
+        <v>161</v>
+      </c>
+      <c r="W1" t="s">
+        <v>162</v>
+      </c>
+      <c r="X1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>164</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>167</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>168</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AH1" t="s">
         <v>173</v>
       </c>
-      <c r="P1" t="s">
+      <c r="AI1" t="s">
         <v>174</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AJ1" t="s">
         <v>175</v>
       </c>
-      <c r="R1" t="s">
+      <c r="AK1" t="s">
         <v>176</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AL1" t="s">
         <v>177</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AM1" t="s">
         <v>178</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AN1" t="s">
         <v>179</v>
-      </c>
-      <c r="V1" t="s">
-        <v>180</v>
-      </c>
-      <c r="W1" t="s">
-        <v>181</v>
-      </c>
-      <c r="X1" t="s">
-        <v>182</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>183</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>184</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>185</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>186</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>187</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>188</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>189</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>190</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>191</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>192</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>193</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>194</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>195</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>196</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>197</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:40">
       <c r="A2" s="1" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="B2">
         <v>256</v>
@@ -5419,7 +5176,7 @@
         <v>12</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="L2" t="s">
         <v>30</v>
@@ -5512,14 +5269,14 @@
   </sheetData>
   <dataValidations count="4">
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="M1 S1 Z1:AN1 Q$1:Q$1048576"/>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
-      <formula1>0</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L$1:L$1048576 M2:M1048576 R$1:R$1048576 S2:S1048576 Z2:AN1048576 T$1:Y$1048576 N$1:P$1048576">
       <formula1>"int,string,float,object"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
+      <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5588,21 +5345,21 @@
         <v>130</v>
       </c>
       <c r="M1" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="N1" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="O1" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="P1" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
       <c r="B2">
         <v>128</v>
@@ -5632,7 +5389,7 @@
         <v>12</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="L2" t="s">
         <v>11</v>
@@ -5652,11 +5409,11 @@
     </row>
   </sheetData>
   <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
       <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
-      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L$1:P$1048576">
       <formula1>"int,string,float,object"</formula1>
@@ -5745,10 +5502,10 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
       <c r="M1" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
       <c r="N1" t="s">
         <v>75</v>
@@ -5825,7 +5582,7 @@
     </row>
     <row r="2" spans="1:37">
       <c r="A2" s="1" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="B2">
         <v>15</v>
@@ -5855,7 +5612,7 @@
         <v>12</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>30</v>
@@ -5938,11 +5695,11 @@
     </row>
   </sheetData>
   <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
       <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
-      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="N$1:AK$1048576">
       <formula1>"int,string,float,object"</formula1>
@@ -6105,7 +5862,7 @@
     </row>
     <row r="2" spans="1:35">
       <c r="A2" s="1" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="B2">
         <v>15</v>
@@ -6135,7 +5892,7 @@
         <v>12</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="L2" t="s">
         <v>15</v>
@@ -6212,11 +5969,11 @@
     </row>
   </sheetData>
   <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
       <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
-      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L$1:AI$1048576">
       <formula1>"int,string,float,object"</formula1>
@@ -6288,21 +6045,21 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="M1" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="N1" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
       <c r="O1" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -6332,7 +6089,7 @@
         <v>12</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="L2" t="s">
         <v>11</v>
@@ -6349,14 +6106,14 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
-      <formula1>0</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L$1:O$1048576">
       <formula1>"int,float,string,object"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
+      <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6423,18 +6180,18 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
       <c r="M1" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="N1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="B2">
         <v>512</v>
@@ -6464,7 +6221,7 @@
         <v>12</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="L2" t="s">
         <v>11</v>
@@ -6478,14 +6235,14 @@
     </row>
   </sheetData>
   <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G42">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D$1:F$1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
       <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G42">
-      <formula1>"true,false"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L$1:M$1048576">
       <formula1>"int,float,string,object"</formula1>

</xml_diff>

<commit_message>
Add Team Switch Server
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
@@ -511,7 +511,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="223">
   <si>
     <t>Id</t>
   </si>
@@ -1305,6 +1305,14 @@
   </si>
   <si>
     <t>DEF_WIND</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>TeamID</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>所在队伍ID</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -1852,10 +1860,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J65"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3947,6 +3955,38 @@
       </c>
       <c r="J65" t="s">
         <v>130</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" t="s">
+        <v>221</v>
+      </c>
+      <c r="B66" t="s">
+        <v>30</v>
+      </c>
+      <c r="C66" t="b">
+        <v>0</v>
+      </c>
+      <c r="D66" t="b">
+        <v>1</v>
+      </c>
+      <c r="E66" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" t="b">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66" t="s">
+        <v>12</v>
+      </c>
+      <c r="J66" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed Record_BagItemList in Player
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/Player.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="19455" windowHeight="9990" firstSheet="5" activeTab="7"/>
+    <workbookView windowWidth="21495" windowHeight="10350" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Property" sheetId="1" r:id="rId1"/>
@@ -40,11 +40,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">物品配置ID</t>
+          <t>物品配置ID</t>
         </r>
       </text>
     </comment>
@@ -53,11 +52,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">强化等级</t>
+          <t>强化等级</t>
         </r>
       </text>
     </comment>
@@ -66,11 +64,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">经验</t>
+          <t>经验</t>
         </r>
       </text>
     </comment>
@@ -79,11 +76,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">星级</t>
+          <t>星级</t>
         </r>
       </text>
     </comment>
@@ -102,11 +98,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">物品配置ID</t>
+          <t>物品配置ID</t>
         </r>
       </text>
     </comment>
@@ -115,11 +110,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">强化等级</t>
+          <t>强化等级</t>
         </r>
       </text>
     </comment>
@@ -128,11 +122,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">镶嵌宝石，逗号分隔</t>
+          <t>镶嵌宝石，逗号分隔</t>
         </r>
       </text>
     </comment>
@@ -141,11 +134,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">附魔等级</t>
+          <t>附魔等级</t>
         </r>
       </text>
     </comment>
@@ -154,11 +146,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">物品配置ID</t>
+          <t>物品配置ID</t>
         </r>
       </text>
     </comment>
@@ -167,11 +158,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">强化等级</t>
+          <t>强化等级</t>
         </r>
       </text>
     </comment>
@@ -180,11 +170,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">镶嵌宝石，逗号分隔</t>
+          <t>镶嵌宝石，逗号分隔</t>
         </r>
       </text>
     </comment>
@@ -193,11 +182,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">附魔等级</t>
+          <t>附魔等级</t>
         </r>
       </text>
     </comment>
@@ -216,11 +204,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">物品配置ID</t>
+          <t>物品配置ID</t>
         </r>
       </text>
     </comment>
@@ -229,11 +216,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">强化等级</t>
+          <t>强化等级</t>
         </r>
       </text>
     </comment>
@@ -242,11 +228,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">镶嵌宝石，逗号分隔</t>
+          <t>镶嵌宝石，逗号分隔</t>
         </r>
       </text>
     </comment>
@@ -255,11 +240,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">附魔等级</t>
+          <t>附魔等级</t>
         </r>
       </text>
     </comment>
@@ -268,11 +252,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">物品配置ID</t>
+          <t>物品配置ID</t>
         </r>
       </text>
     </comment>
@@ -281,11 +264,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">强化等级</t>
+          <t>强化等级</t>
         </r>
       </text>
     </comment>
@@ -294,11 +276,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">镶嵌宝石，逗号分隔</t>
+          <t>镶嵌宝石，逗号分隔</t>
         </r>
       </text>
     </comment>
@@ -307,11 +288,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">附魔等级</t>
+          <t>附魔等级</t>
         </r>
       </text>
     </comment>
@@ -330,11 +310,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">物品配置ID</t>
+          <t>物品配置ID</t>
         </r>
       </text>
     </comment>
@@ -343,11 +322,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">强化等级</t>
+          <t>强化等级</t>
         </r>
       </text>
     </comment>
@@ -356,11 +334,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">镶嵌宝石，逗号分隔</t>
+          <t>镶嵌宝石，逗号分隔</t>
         </r>
       </text>
     </comment>
@@ -369,11 +346,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">附魔等级</t>
+          <t>附魔等级</t>
         </r>
       </text>
     </comment>
@@ -392,11 +368,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">任务ID</t>
+          <t>任务ID</t>
         </r>
       </text>
     </comment>
@@ -405,11 +380,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">任务状态，见NFDefine.proto中ETaskState</t>
+          <t>任务状态，见NFDefine.proto中ETaskState</t>
         </r>
       </text>
     </comment>
@@ -418,11 +392,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">当前进度</t>
+          <t>当前进度</t>
         </r>
       </text>
     </comment>
@@ -441,11 +414,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">建筑ID</t>
+          <t>建筑ID</t>
         </r>
       </text>
     </comment>
@@ -464,11 +436,10 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">建筑ID</t>
+          <t>建筑ID</t>
         </r>
       </text>
     </comment>
@@ -1263,10 +1234,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -1314,26 +1285,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1352,8 +1323,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1361,6 +1341,37 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1374,42 +1385,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1422,23 +1402,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1483,7 +1454,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1501,7 +1526,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1513,61 +1586,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1579,49 +1598,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1633,25 +1610,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1662,60 +1633,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1743,6 +1660,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1762,99 +1709,123 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1863,52 +1834,52 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2013,7 +1984,7 @@
   <dxfs count="2">
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -4651,18 +4622,18 @@
   </sheetData>
   <dataValidations count="6">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="L1:M1 O1:Q1 L42:L1048576"/>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="M2 O2:Q2 L2:L41">
       <formula1>"int,float,string,object"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
-      <formula1>0</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2">
       <formula1>"int,float,string,object"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
-      <formula1>"TRUE,FALSE"</formula1>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
+      <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4814,18 +4785,18 @@
   </sheetData>
   <dataValidations count="6">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="L1:M1 O1:Q1 L42:L1048576"/>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="M2 O2:Q2 L2:L41">
       <formula1>"int,float,string,object"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
-      <formula1>0</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2">
       <formula1>"int,float,string,object"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
-      <formula1>"TRUE,FALSE"</formula1>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
+      <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5477,10 +5448,10 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="M1 R1 Y1:AH1 Q$1:Q$1048576"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="M1 R1 Y1:AH1 Q$1:Q$1048576"/>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L$1:L$1048576 M2:M1048576 R2:R1048576 Y2:AH1048576 S$1:X$1048576 N$1:P$1048576">
       <formula1>"int,string,float,object"</formula1>
     </dataValidation>
@@ -5497,10 +5468,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -5511,12 +5482,12 @@
     <col min="5" max="5" width="11.625" customWidth="1"/>
     <col min="8" max="8" width="9.375" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="12" max="12" width="12.75" customWidth="1"/>
-    <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="15" max="15" width="16.5" customWidth="1"/>
+    <col min="13" max="13" width="12.75" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="16" max="16" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5551,22 +5522,25 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
+        <v>141</v>
+      </c>
+      <c r="M1" t="s">
         <v>142</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>188</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>189</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>166</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
         <v>190</v>
       </c>
@@ -5600,12 +5574,12 @@
       <c r="K2" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" t="s">
-        <v>15</v>
-      </c>
       <c r="N2" t="s">
         <v>15</v>
       </c>
@@ -5613,7 +5587,10 @@
         <v>15</v>
       </c>
       <c r="P2" t="s">
-        <v>30</v>
+        <v>15</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -5621,11 +5598,11 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L$1:P$1048576">
-      <formula1>"int,string,float,object"</formula1>
-    </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
       <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="M$1:Q$1048576">
+      <formula1>"int,string,float,object"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6258,7 +6235,7 @@
   <sheetPr/>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16:I17"/>
     </sheetView>
   </sheetViews>
@@ -6502,17 +6479,17 @@
     </row>
   </sheetData>
   <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G42">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G42">
-      <formula1>"true,false"</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L$1:M$1048576">
+      <formula1>"int,float,string,object"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D$1:F$1048576">
       <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L$1:M$1048576">
-      <formula1>"int,float,string,object"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>